<commit_message>
Fin journée mission wz
</commit_message>
<xml_diff>
--- a/mission wz.xlsx
+++ b/mission wz.xlsx
@@ -126,19 +126,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="25">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <condense val="0"/>
@@ -160,210 +148,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -719,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -779,7 +563,7 @@
       </c>
       <c r="C2" s="4">
         <f>(150000-C6)/150000</f>
-        <v>0.11648</v>
+        <v>0.1168</v>
       </c>
       <c r="D2" s="4">
         <f t="shared" ref="D2" si="0">(150-D6)/150</f>
@@ -791,11 +575,11 @@
       </c>
       <c r="F2" s="4">
         <f t="shared" ref="F2" si="2">(150-F6)/150</f>
-        <v>0.11333333333333333</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="G2" s="4">
         <f t="shared" ref="G2" si="3">(150000-G6)/150000</f>
-        <v>0.11896666666666667</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="H2" s="4">
         <f t="shared" ref="H2" si="4">(150-H6)/150</f>
@@ -803,7 +587,7 @@
       </c>
       <c r="I2" s="4">
         <f t="shared" ref="I2" si="5">(150000-I6)/150000</f>
-        <v>0.11177333333333334</v>
+        <v>0.11647333333333333</v>
       </c>
       <c r="J2" s="4">
         <f t="shared" ref="J2" si="6">(150-J6)/150</f>
@@ -815,19 +599,19 @@
       </c>
       <c r="L2" s="4">
         <f t="shared" ref="L2" si="8">(150-L6)/150</f>
-        <v>6.6666666666666666E-2</v>
+        <v>7.3333333333333334E-2</v>
       </c>
       <c r="M2" s="4">
         <f t="shared" ref="M2" si="9">(150000-M6)/150000</f>
-        <v>4.5333333333333337E-2</v>
+        <v>7.6293333333333338E-2</v>
       </c>
       <c r="N2" s="4">
         <f t="shared" ref="N2" si="10">(150-N6)/150</f>
-        <v>8.666666666666667E-2</v>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="O2" s="4">
         <f t="shared" ref="O2" si="11">(150000-O6)/150000</f>
-        <v>0.13410666666666668</v>
+        <v>0.15672666666666665</v>
       </c>
       <c r="Q2" s="3">
         <v>41989</v>
@@ -850,7 +634,7 @@
       </c>
       <c r="C3" s="1">
         <f ca="1">INT(C6/$S$1)</f>
-        <v>4569</v>
+        <v>4568</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:O3" ca="1" si="12">INT(D6/$S$1)</f>
@@ -866,7 +650,7 @@
       </c>
       <c r="G3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4557</v>
+        <v>4468</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -874,7 +658,7 @@
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4594</v>
+        <v>4569</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -890,7 +674,7 @@
       </c>
       <c r="M3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4937</v>
+        <v>4777</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -898,7 +682,7 @@
       </c>
       <c r="O3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4478</v>
+        <v>4361</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" t="s">
@@ -919,7 +703,7 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:O4" si="13">C9-C10</f>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="13"/>
@@ -931,11 +715,11 @@
       </c>
       <c r="F4" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2555</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="13"/>
@@ -943,7 +727,7 @@
       </c>
       <c r="I4" s="2">
         <f t="shared" si="13"/>
-        <v>849</v>
+        <v>1554</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="13"/>
@@ -955,19 +739,19 @@
       </c>
       <c r="L4" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>4644</v>
       </c>
       <c r="N4" s="2">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="13"/>
-        <v>337</v>
+        <v>3730</v>
       </c>
       <c r="Q4" s="3"/>
     </row>
@@ -981,7 +765,7 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">150000-INT(150000-150000/34*$S$1)-C6</f>
-        <v>-4586</v>
+        <v>-4538</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ref="D5" ca="1" si="14">150-INT(150-150/34*$S$1)-D6</f>
@@ -993,11 +777,11 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5" ca="1" si="16">150-INT(150-150/34*$S$1)-F6</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" ref="G5" ca="1" si="17">150000-INT(150000-150000/34*$S$1)-G6</f>
-        <v>-4213</v>
+        <v>-1658</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5" ca="1" si="18">150-INT(150-150/34*$S$1)-H6</f>
@@ -1005,7 +789,7 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5" ca="1" si="19">150000-INT(150000-150000/34*$S$1)-I6</f>
-        <v>-5292</v>
+        <v>-4587</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ref="J5" ca="1" si="20">150-INT(150-150/34*$S$1)-J6</f>
@@ -1017,35 +801,35 @@
       </c>
       <c r="L5" s="1">
         <f t="shared" ref="L5" ca="1" si="22">150-INT(150-150/34*$S$1)-L6</f>
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="M5" s="1">
         <f t="shared" ref="M5" ca="1" si="23">150000-INT(150000-150000/34*$S$1)-M6</f>
-        <v>-15258</v>
+        <v>-10614</v>
       </c>
       <c r="N5" s="1">
         <f t="shared" ref="N5" ca="1" si="24">150-INT(150-150/34*$S$1)-N6</f>
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" ref="O5" ca="1" si="25">150000-INT(150000-150000/34*$S$1)-O6</f>
-        <v>-1942</v>
+        <v>1451</v>
       </c>
       <c r="P5">
         <f ca="1">SUM(B5,D5,F5,H5,J5,L5,N5)</f>
-        <v>-66</v>
+        <v>-62</v>
       </c>
       <c r="Q5">
         <f ca="1">SUM(C5,E5,G5,I5,K5,M5,O5)</f>
-        <v>-72820</v>
+        <v>-61475</v>
       </c>
       <c r="R5" s="5">
         <f ca="1">-$S$3+R6</f>
-        <v>-3.740259740259741E-2</v>
+        <v>-3.3593073593073591E-2</v>
       </c>
       <c r="S5" s="5">
         <f ca="1">-$S$3+S6</f>
-        <v>-4.3511168831168831E-2</v>
+        <v>-3.2706406926406931E-2</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1058,7 +842,7 @@
       </c>
       <c r="C6" s="1">
         <f>150000-C9</f>
-        <v>132528</v>
+        <v>132480</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6" si="26">150-D9</f>
@@ -1070,11 +854,11 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6" si="28">150-F9</f>
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ref="G6" si="29">150000-G9</f>
-        <v>132155</v>
+        <v>129600</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6" si="30">150-H9</f>
@@ -1082,7 +866,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" ref="I6" si="31">150000-I9</f>
-        <v>133234</v>
+        <v>132529</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" ref="J6" si="32">150-J9</f>
@@ -1094,35 +878,35 @@
       </c>
       <c r="L6" s="1">
         <f t="shared" ref="L6" si="34">150-L9</f>
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" ref="M6" si="35">150000-M9</f>
-        <v>143200</v>
+        <v>138556</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" ref="N6" si="36">150-N9</f>
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" ref="O6" si="37">150000-O9</f>
-        <v>129884</v>
+        <v>126491</v>
       </c>
       <c r="P6">
         <f>SUM(B6,D6,F6,H6,J6,L6,N6)</f>
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="Q6">
         <f>SUM(C6,E6,G6,I6,K6,M6,O6)</f>
-        <v>968414</v>
+        <v>957069</v>
       </c>
       <c r="R6" s="5">
         <f>(7*150-P6)/(7*150)</f>
-        <v>8.3809523809523806E-2</v>
+        <v>8.7619047619047624E-2</v>
       </c>
       <c r="S6" s="5">
         <f>(7*150000-Q6)/(7*150000)</f>
-        <v>7.7700952380952384E-2</v>
+        <v>8.8505714285714285E-2</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1145,11 +929,11 @@
       <c r="O7" s="1"/>
       <c r="P7">
         <f>150*7-P6</f>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="Q7">
         <f>150000*7-Q6</f>
-        <v>81586</v>
+        <v>92931</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -1207,11 +991,10 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:O9" si="38">C10</f>
-        <v>17472</v>
+        <v>17520</v>
       </c>
       <c r="D9">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="C9:M9" si="38">D10</f>
         <v>0</v>
       </c>
       <c r="E9">
@@ -1219,18 +1002,16 @@
         <v>2587</v>
       </c>
       <c r="F9">
-        <f t="shared" si="38"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G9">
-        <f t="shared" si="38"/>
-        <v>17845</v>
+        <v>20400</v>
       </c>
       <c r="H9">
         <v>25</v>
       </c>
       <c r="I9">
-        <v>16766</v>
+        <v>17471</v>
       </c>
       <c r="J9">
         <f t="shared" si="38"/>
@@ -1241,18 +1022,16 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <f t="shared" si="38"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M9">
-        <f t="shared" si="38"/>
-        <v>6800</v>
+        <v>11444</v>
       </c>
       <c r="N9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O9">
-        <v>20116</v>
+        <v>23509</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1266,7 +1045,7 @@
         <v>17472</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D9:K11" si="39">D11</f>
+        <f t="shared" ref="D10:K11" si="39">D11</f>
         <v>0</v>
       </c>
       <c r="E10">
@@ -1412,33 +1191,33 @@
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:O5">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="greaterThan">
       <formula>$S$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:O2">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>$S$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:O2">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>$S$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5:S5">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
début combat : 10h
</commit_message>
<xml_diff>
--- a/mission wz.xlsx
+++ b/mission wz.xlsx
@@ -107,7 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,6 +119,9 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -503,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -557,61 +560,61 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="7">
         <f>(150-B6)/150</f>
         <v>0.15333333333333332</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="7">
         <f>(150000-C6)/150000</f>
-        <v>0.1168</v>
-      </c>
-      <c r="D2" s="4">
+        <v>0.11733333333333333</v>
+      </c>
+      <c r="D2" s="7">
         <f t="shared" ref="D2" si="0">(150-D6)/150</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="4">
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="E2" s="7">
         <f t="shared" ref="E2" si="1">(150000-E6)/150000</f>
-        <v>1.7246666666666667E-2</v>
-      </c>
-      <c r="F2" s="4">
+        <v>3.914666666666667E-2</v>
+      </c>
+      <c r="F2" s="7">
         <f t="shared" ref="F2" si="2">(150-F6)/150</f>
         <v>0.12666666666666668</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="7">
         <f t="shared" ref="G2" si="3">(150000-G6)/150000</f>
         <v>0.13600000000000001</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="7">
         <f t="shared" ref="H2" si="4">(150-H6)/150</f>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="I2" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I2" s="7">
         <f t="shared" ref="I2" si="5">(150000-I6)/150000</f>
-        <v>0.11647333333333333</v>
-      </c>
-      <c r="J2" s="4">
+        <v>0.13942666666666667</v>
+      </c>
+      <c r="J2" s="7">
         <f t="shared" ref="J2" si="6">(150-J6)/150</f>
         <v>0</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="7">
         <f t="shared" ref="K2" si="7">(150000-K6)/150000</f>
         <v>0</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="7">
         <f t="shared" ref="L2" si="8">(150-L6)/150</f>
         <v>7.3333333333333334E-2</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="7">
         <f t="shared" ref="M2" si="9">(150000-M6)/150000</f>
         <v>7.6293333333333338E-2</v>
       </c>
-      <c r="N2" s="4">
+      <c r="N2" s="7">
         <f t="shared" ref="N2" si="10">(150-N6)/150</f>
-        <v>9.3333333333333338E-2</v>
-      </c>
-      <c r="O2" s="4">
+        <v>0.10666666666666667</v>
+      </c>
+      <c r="O2" s="7">
         <f t="shared" ref="O2" si="11">(150000-O6)/150000</f>
-        <v>0.15672666666666665</v>
+        <v>0.18071333333333334</v>
       </c>
       <c r="Q2" s="3">
         <v>41989</v>
@@ -634,7 +637,7 @@
       </c>
       <c r="C3" s="1">
         <f ca="1">INT(C6/$S$1)</f>
-        <v>4568</v>
+        <v>4565</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:O3" ca="1" si="12">INT(D6/$S$1)</f>
@@ -642,7 +645,7 @@
       </c>
       <c r="E3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>5083</v>
+        <v>4969</v>
       </c>
       <c r="F3" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -658,7 +661,7 @@
       </c>
       <c r="I3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4569</v>
+        <v>4451</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ca="1" si="12"/>
@@ -682,7 +685,7 @@
       </c>
       <c r="O3" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>4361</v>
+        <v>4237</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" t="s">
@@ -703,15 +706,15 @@
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:O4" si="13">C9-C10</f>
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>3285</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="13"/>
@@ -723,11 +726,11 @@
       </c>
       <c r="H4" s="2">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="13"/>
-        <v>1554</v>
+        <v>4997</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="13"/>
@@ -747,11 +750,11 @@
       </c>
       <c r="N4" s="2">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O4" s="2">
         <f t="shared" si="13"/>
-        <v>3730</v>
+        <v>7328</v>
       </c>
       <c r="Q4" s="3"/>
     </row>
@@ -765,15 +768,15 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">150000-INT(150000-150000/34*$S$1)-C6</f>
-        <v>-4538</v>
+        <v>-4458</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" ref="D5" ca="1" si="14">150-INT(150-150/34*$S$1)-D6</f>
-        <v>-22</v>
+        <v>-20</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5" ca="1" si="15">150000-INT(150000-150000/34*$S$1)-E6</f>
-        <v>-19471</v>
+        <v>-16186</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" ref="F5" ca="1" si="16">150-INT(150-150/34*$S$1)-F6</f>
@@ -785,11 +788,11 @@
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5" ca="1" si="18">150-INT(150-150/34*$S$1)-H6</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" ref="I5" ca="1" si="19">150000-INT(150000-150000/34*$S$1)-I6</f>
-        <v>-4587</v>
+        <v>-1144</v>
       </c>
       <c r="J5" s="1">
         <f t="shared" ref="J5" ca="1" si="20">150-INT(150-150/34*$S$1)-J6</f>
@@ -809,27 +812,27 @@
       </c>
       <c r="N5" s="1">
         <f t="shared" ref="N5" ca="1" si="24">150-INT(150-150/34*$S$1)-N6</f>
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" ref="O5" ca="1" si="25">150000-INT(150000-150000/34*$S$1)-O6</f>
-        <v>1451</v>
+        <v>5049</v>
       </c>
       <c r="P5">
         <f ca="1">SUM(B5,D5,F5,H5,J5,L5,N5)</f>
-        <v>-62</v>
+        <v>-53</v>
       </c>
       <c r="Q5">
         <f ca="1">SUM(C5,E5,G5,I5,K5,M5,O5)</f>
-        <v>-61475</v>
+        <v>-51069</v>
       </c>
       <c r="R5" s="5">
         <f ca="1">-$S$3+R6</f>
-        <v>-3.3593073593073591E-2</v>
+        <v>-2.5021645021645028E-2</v>
       </c>
       <c r="S5" s="5">
         <f ca="1">-$S$3+S6</f>
-        <v>-3.2706406926406931E-2</v>
+        <v>-2.2795930735930739E-2</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -842,15 +845,15 @@
       </c>
       <c r="C6" s="1">
         <f>150000-C9</f>
-        <v>132480</v>
+        <v>132400</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6" si="26">150-D9</f>
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" ref="E6" si="27">150000-E9</f>
-        <v>147413</v>
+        <v>144128</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" ref="F6" si="28">150-F9</f>
@@ -862,11 +865,11 @@
       </c>
       <c r="H6" s="1">
         <f t="shared" ref="H6" si="30">150-H9</f>
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" ref="I6" si="31">150000-I9</f>
-        <v>132529</v>
+        <v>129086</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" ref="J6" si="32">150-J9</f>
@@ -886,27 +889,27 @@
       </c>
       <c r="N6" s="1">
         <f t="shared" ref="N6" si="36">150-N9</f>
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" ref="O6" si="37">150000-O9</f>
-        <v>126491</v>
+        <v>122893</v>
       </c>
       <c r="P6">
         <f>SUM(B6,D6,F6,H6,J6,L6,N6)</f>
-        <v>958</v>
+        <v>949</v>
       </c>
       <c r="Q6">
         <f>SUM(C6,E6,G6,I6,K6,M6,O6)</f>
-        <v>957069</v>
+        <v>946663</v>
       </c>
       <c r="R6" s="5">
         <f>(7*150-P6)/(7*150)</f>
-        <v>8.7619047619047624E-2</v>
+        <v>9.6190476190476187E-2</v>
       </c>
       <c r="S6" s="5">
         <f>(7*150000-Q6)/(7*150000)</f>
-        <v>8.8505714285714285E-2</v>
+        <v>9.8416190476190477E-2</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -929,11 +932,11 @@
       <c r="O7" s="1"/>
       <c r="P7">
         <f>150*7-P6</f>
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="Q7">
         <f>150000*7-Q6</f>
-        <v>92931</v>
+        <v>103337</v>
       </c>
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
@@ -991,15 +994,13 @@
         <v>23</v>
       </c>
       <c r="C9">
-        <v>17520</v>
+        <v>17600</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="C9:M9" si="38">D10</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9">
-        <f t="shared" si="38"/>
-        <v>2587</v>
+        <v>5872</v>
       </c>
       <c r="F9">
         <v>19</v>
@@ -1008,13 +1009,13 @@
         <v>20400</v>
       </c>
       <c r="H9">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I9">
-        <v>17471</v>
+        <v>20914</v>
       </c>
       <c r="J9">
-        <f t="shared" si="38"/>
+        <f t="shared" ref="D9:K9" si="38">J10</f>
         <v>0</v>
       </c>
       <c r="K9">
@@ -1028,10 +1029,18 @@
         <v>11444</v>
       </c>
       <c r="N9">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O9">
-        <v>23509</v>
+        <v>27107</v>
+      </c>
+      <c r="P9">
+        <f>SUM(B9,D9,F9,H9,J9,L9,N9)-SUM(B10,D10,F10,H10,J10,L10,N10)</f>
+        <v>17</v>
+      </c>
+      <c r="Q9">
+        <f>SUM(C9,E9,G9,I9,K9,M9,O9)-SUM(C10,E10,G10,I10,K10,M10,O10)</f>
+        <v>22937</v>
       </c>
     </row>
     <row r="10" spans="1:19">
@@ -1082,6 +1091,14 @@
       <c r="O10">
         <v>19779</v>
       </c>
+      <c r="P10">
+        <f t="shared" ref="P10:P12" si="40">SUM(B10,D10,F10,H10,J10,L10,N10)-SUM(B11,D11,F11,H11,J11,L11,N11)</f>
+        <v>17</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ref="Q10:Q12" si="41">SUM(C10,E10,G10,I10,K10,M10,O10)-SUM(C11,E11,G11,I11,K11,M11,O11)</f>
+        <v>20059</v>
+      </c>
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="3">
@@ -1132,6 +1149,14 @@
       <c r="O11">
         <v>11237</v>
       </c>
+      <c r="P11">
+        <f t="shared" si="40"/>
+        <v>28</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="41"/>
+        <v>18859</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="3">
@@ -1178,6 +1203,14 @@
       </c>
       <c r="O12">
         <v>9358</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="40"/>
+        <v>39</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="41"/>
+        <v>41482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maj 21/12/2014 à 21h
</commit_message>
<xml_diff>
--- a/mission wz.xlsx
+++ b/mission wz.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t>France</t>
   </si>
@@ -75,9 +75,6 @@
     <t>dKill Total</t>
   </si>
   <si>
-    <t>ddég total</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -100,6 +97,15 @@
   </si>
   <si>
     <t>Vendredi</t>
+  </si>
+  <si>
+    <t>Partie fin de journée</t>
+  </si>
+  <si>
+    <t>dDég total</t>
+  </si>
+  <si>
+    <t>tot partie</t>
   </si>
 </sst>
 </file>
@@ -272,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -301,6 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,7 +679,7 @@
   <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+      <selection activeCell="AG42" sqref="AG42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -754,7 +761,7 @@
       <c r="AC1" s="19"/>
       <c r="AD1" s="19"/>
       <c r="AE1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AI1" s="1">
         <f ca="1">TODAY()</f>
@@ -788,37 +795,37 @@
       </c>
       <c r="H2" s="8">
         <f t="shared" ref="H2" si="1">(150000-H6)/150000</f>
-        <v>7.8E-2</v>
+        <v>7.8573333333333328E-2</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8">
         <f t="shared" ref="K2" si="2">(150-K6)/150</f>
-        <v>0.2</v>
+        <v>0.25333333333333335</v>
       </c>
       <c r="L2" s="8">
         <f t="shared" ref="L2" si="3">(150000-L6)/150000</f>
-        <v>0.21236666666666668</v>
+        <v>0.25908666666666669</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f t="shared" ref="O2" si="4">(150-O6)/150</f>
-        <v>0.26666666666666666</v>
+        <v>0.29333333333333333</v>
       </c>
       <c r="P2" s="8">
         <f t="shared" ref="P2" si="5">(150000-P6)/150000</f>
-        <v>0.18141333333333334</v>
+        <v>0.20826666666666666</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8">
         <f t="shared" ref="S2" si="6">(150-S6)/150</f>
-        <v>4.6666666666666669E-2</v>
+        <v>0.08</v>
       </c>
       <c r="T2" s="8">
         <f t="shared" ref="T2" si="7">(150000-T6)/150000</f>
-        <v>2.2006666666666667E-2</v>
+        <v>5.3273333333333332E-2</v>
       </c>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
@@ -828,17 +835,17 @@
       </c>
       <c r="X2" s="8">
         <f t="shared" ref="X2" si="9">(150000-X6)/150000</f>
-        <v>0.18218000000000001</v>
+        <v>0.19066</v>
       </c>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8">
         <f t="shared" ref="AA2" si="10">(150-AA6)/150</f>
-        <v>0.18</v>
+        <v>0.19333333333333333</v>
       </c>
       <c r="AB2" s="8">
         <f t="shared" ref="AB2" si="11">(150000-AB6)/150000</f>
-        <v>0.28491333333333335</v>
+        <v>0.32140000000000002</v>
       </c>
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
@@ -871,7 +878,7 @@
       </c>
       <c r="H3" s="9">
         <f ca="1">INT(H6/$AK$1)</f>
-        <v>4939</v>
+        <v>4936</v>
       </c>
       <c r="K3" s="9">
         <f ca="1">INT(K6/$AK$1)</f>
@@ -879,7 +886,7 @@
       </c>
       <c r="L3" s="9">
         <f ca="1">INT(L6/$AK$1)</f>
-        <v>4219</v>
+        <v>3969</v>
       </c>
       <c r="O3" s="9">
         <f ca="1">INT(O6/$AK$1)</f>
@@ -887,15 +894,15 @@
       </c>
       <c r="P3" s="9">
         <f ca="1">INT(P6/$AK$1)</f>
-        <v>4385</v>
+        <v>4241</v>
       </c>
       <c r="S3" s="9">
         <f ca="1">INT(S6/$AK$1)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T3" s="9">
         <f ca="1">INT(T6/$AK$1)</f>
-        <v>5239</v>
+        <v>5071</v>
       </c>
       <c r="W3" s="9">
         <f ca="1">INT(W6/$AK$1)</f>
@@ -903,7 +910,7 @@
       </c>
       <c r="X3" s="9">
         <f ca="1">INT(X6/$AK$1)</f>
-        <v>4381</v>
+        <v>4335</v>
       </c>
       <c r="AA3" s="9">
         <f ca="1">INT(AA6/$AK$1)</f>
@@ -911,15 +918,15 @@
       </c>
       <c r="AB3" s="9">
         <f ca="1">INT(AB6/$AK$1)</f>
-        <v>3830</v>
+        <v>3635</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE4" ca="1" si="12">SUM(C3,G3,K3,O3,S3,W3,AA3)</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AF3" s="5">
         <f ca="1">SUM(D3,H3,L3,P3,T3,X3,AB3)</f>
-        <v>31368</v>
+        <v>30562</v>
       </c>
       <c r="AI3" s="1">
         <v>41996</v>
@@ -1019,31 +1026,31 @@
       </c>
       <c r="H5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-H6</f>
-        <v>-14770</v>
+        <v>-14684</v>
       </c>
       <c r="K5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-K6</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="L5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-L6</f>
-        <v>5385</v>
+        <v>12393</v>
       </c>
       <c r="O5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-O6</f>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="P5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-P6</f>
-        <v>742</v>
+        <v>4770</v>
       </c>
       <c r="S5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-S6</f>
-        <v>-19</v>
+        <v>-14</v>
       </c>
       <c r="T5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-T6</f>
-        <v>-23169</v>
+        <v>-18479</v>
       </c>
       <c r="W5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-W6</f>
@@ -1051,31 +1058,31 @@
       </c>
       <c r="X5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-X6</f>
-        <v>857</v>
+        <v>2129</v>
       </c>
       <c r="AA5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-AA6</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-AB6</f>
-        <v>16267</v>
+        <v>21740</v>
       </c>
       <c r="AE5" s="5">
         <f ca="1">SUM(C5,G5,K5,O5,S5,W5,AA5)</f>
-        <v>-7</v>
+        <v>12</v>
       </c>
       <c r="AF5" s="5">
         <f ca="1">SUM(D5,H5,L5,P5,T5,X5,AB5)</f>
-        <v>-13666</v>
+        <v>8891</v>
       </c>
       <c r="AG5" s="3">
         <f ca="1">-$AK$3+AG6</f>
-        <v>1.5151515151515138E-2</v>
+        <v>3.3246753246753247E-2</v>
       </c>
       <c r="AH5" s="3">
         <f ca="1">AH6-$AK$3</f>
-        <v>1.1936277056277061E-2</v>
+        <v>3.3419134199134198E-2</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -1096,31 +1103,31 @@
       </c>
       <c r="H6" s="9">
         <f>150000-H11</f>
-        <v>138300</v>
+        <v>138214</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" ref="K6" si="15">150-K11</f>
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="L6" s="9">
         <f>150000-L11</f>
-        <v>118145</v>
+        <v>111137</v>
       </c>
       <c r="O6" s="9">
         <f t="shared" ref="O6" si="16">150-O11</f>
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P6" s="9">
         <f>150000-P11</f>
-        <v>122788</v>
+        <v>118760</v>
       </c>
       <c r="S6" s="9">
         <f t="shared" ref="S6" si="17">150-S11</f>
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="T6" s="9">
         <f>150000-T11</f>
-        <v>146699</v>
+        <v>142009</v>
       </c>
       <c r="W6" s="9">
         <f t="shared" ref="W6" si="18">150-W11</f>
@@ -1128,31 +1135,31 @@
       </c>
       <c r="X6" s="9">
         <f>150000-X11</f>
-        <v>122673</v>
+        <v>121401</v>
       </c>
       <c r="AA6" s="9">
         <f t="shared" ref="AA6" si="19">150-AA11</f>
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="AB6" s="9">
         <f>150000-AB11</f>
-        <v>107263</v>
+        <v>101790</v>
       </c>
       <c r="AE6" s="5">
         <f>SUM(C6,G6,K6,O6,S6,W6,AA6)</f>
-        <v>875</v>
+        <v>856</v>
       </c>
       <c r="AF6" s="5">
         <f>SUM(D6,H6,L6,P6,T6,X6,AB6)</f>
-        <v>878376</v>
+        <v>855819</v>
       </c>
       <c r="AG6" s="3">
         <f>(7*150-AE6)/(7*150)</f>
-        <v>0.16666666666666666</v>
+        <v>0.18476190476190477</v>
       </c>
       <c r="AH6" s="3">
         <f>(7*150000-AF6)/(7*150000)</f>
-        <v>0.16345142857142858</v>
+        <v>0.18493428571428572</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -1161,11 +1168,11 @@
       </c>
       <c r="AE7" s="5">
         <f>150*7-AE6</f>
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="AF7" s="5">
         <f>150000*7-AF6</f>
-        <v>171624</v>
+        <v>194181</v>
       </c>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
@@ -1267,12 +1274,18 @@
         <v>18</v>
       </c>
       <c r="AF10" s="6" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="AG10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH10" s="20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:37" hidden="1">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7">
         <v>42023</v>
@@ -1299,7 +1312,7 @@
       </c>
       <c r="H11" s="14">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I11" s="14">
         <f t="shared" si="20"/>
@@ -1307,87 +1320,87 @@
       </c>
       <c r="J11" s="15">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K11" s="13">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L11" s="14">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M11" s="14">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N11" s="15">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O11" s="13">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R11" s="15">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S11" s="13">
         <f t="shared" ref="S11:AD32" si="21">S12</f>
+        <v>12</v>
+      </c>
+      <c r="T11" s="14">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U11" s="14">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V11" s="15">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W11" s="13">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X11" s="14">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y11" s="14">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z11" s="15">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA11" s="13">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB11" s="14">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC11" s="14">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T11" s="14">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U11" s="14">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V11" s="15">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W11" s="13">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X11" s="14">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y11" s="14">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z11" s="15">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA11" s="13">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB11" s="14">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC11" s="14">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD11" s="15">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE11" s="4">
         <f>SUM(C11,G11,K11,O11,S11,W11,AA11)-SUM(C12,G12,K12,O12,S12,W12,AA12)</f>
@@ -1400,7 +1413,7 @@
     </row>
     <row r="12" spans="1:37" hidden="1">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7">
         <v>42022</v>
@@ -1427,7 +1440,7 @@
       </c>
       <c r="H12" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I12" s="17">
         <f t="shared" si="20"/>
@@ -1435,87 +1448,87 @@
       </c>
       <c r="J12" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K12" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L12" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M12" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N12" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O12" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P12" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q12" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R12" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S12" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T12" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U12" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V12" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W12" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X12" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y12" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z12" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA12" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB12" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC12" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T12" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U12" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V12" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W12" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X12" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y12" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z12" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA12" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB12" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC12" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD12" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE12" s="4">
         <f t="shared" ref="AE12:AF27" si="22">SUM(C12,G12,K12,O12,S12,W12,AA12)-SUM(C13,G13,K13,O13,S13,W13,AA13)</f>
@@ -1528,7 +1541,7 @@
     </row>
     <row r="13" spans="1:37" hidden="1">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="7">
         <v>42021</v>
@@ -1555,7 +1568,7 @@
       </c>
       <c r="H13" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I13" s="17">
         <f t="shared" si="20"/>
@@ -1563,87 +1576,87 @@
       </c>
       <c r="J13" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K13" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L13" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M13" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N13" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O13" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P13" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q13" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R13" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S13" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T13" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U13" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V13" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W13" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X13" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y13" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z13" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA13" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB13" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC13" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T13" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U13" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V13" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W13" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X13" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y13" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z13" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA13" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB13" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC13" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD13" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE13" s="4">
         <f t="shared" si="22"/>
@@ -1656,7 +1669,7 @@
     </row>
     <row r="14" spans="1:37" hidden="1">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7">
         <v>42020</v>
@@ -1683,7 +1696,7 @@
       </c>
       <c r="H14" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I14" s="17">
         <f t="shared" si="20"/>
@@ -1691,87 +1704,87 @@
       </c>
       <c r="J14" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K14" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L14" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M14" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N14" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O14" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P14" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q14" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R14" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S14" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T14" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U14" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V14" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W14" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X14" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y14" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z14" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA14" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB14" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC14" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T14" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U14" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V14" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W14" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X14" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y14" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z14" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA14" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB14" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC14" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD14" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE14" s="4">
         <f t="shared" si="22"/>
@@ -1784,7 +1797,7 @@
     </row>
     <row r="15" spans="1:37" hidden="1">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="7">
         <v>42019</v>
@@ -1811,7 +1824,7 @@
       </c>
       <c r="H15" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I15" s="17">
         <f t="shared" si="20"/>
@@ -1819,87 +1832,87 @@
       </c>
       <c r="J15" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K15" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L15" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M15" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O15" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P15" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q15" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R15" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S15" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T15" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U15" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V15" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W15" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X15" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y15" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z15" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA15" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB15" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC15" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T15" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U15" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V15" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W15" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X15" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y15" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z15" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA15" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB15" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC15" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD15" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE15" s="4">
         <f t="shared" si="22"/>
@@ -1912,7 +1925,7 @@
     </row>
     <row r="16" spans="1:37" hidden="1">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="7">
         <v>42018</v>
@@ -1939,7 +1952,7 @@
       </c>
       <c r="H16" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I16" s="17">
         <f t="shared" si="20"/>
@@ -1947,87 +1960,87 @@
       </c>
       <c r="J16" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K16" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L16" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M16" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N16" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O16" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P16" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q16" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R16" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S16" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T16" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U16" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V16" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W16" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X16" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y16" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z16" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA16" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB16" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC16" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T16" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U16" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V16" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W16" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X16" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y16" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z16" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA16" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB16" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC16" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD16" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE16" s="4">
         <f t="shared" si="22"/>
@@ -2040,7 +2053,7 @@
     </row>
     <row r="17" spans="1:32" hidden="1">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="7">
         <v>42017</v>
@@ -2067,7 +2080,7 @@
       </c>
       <c r="H17" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I17" s="17">
         <f t="shared" si="20"/>
@@ -2075,87 +2088,87 @@
       </c>
       <c r="J17" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K17" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L17" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M17" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N17" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O17" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P17" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q17" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R17" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S17" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T17" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U17" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V17" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W17" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X17" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y17" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z17" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA17" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB17" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC17" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T17" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U17" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V17" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W17" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X17" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y17" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z17" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA17" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB17" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC17" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD17" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE17" s="4">
         <f t="shared" si="22"/>
@@ -2168,7 +2181,7 @@
     </row>
     <row r="18" spans="1:32" hidden="1">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="7">
         <v>42016</v>
@@ -2195,7 +2208,7 @@
       </c>
       <c r="H18" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I18" s="17">
         <f t="shared" si="20"/>
@@ -2203,87 +2216,87 @@
       </c>
       <c r="J18" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K18" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L18" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M18" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N18" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O18" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P18" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q18" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R18" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S18" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T18" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U18" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V18" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W18" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X18" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y18" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z18" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA18" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB18" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC18" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T18" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U18" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V18" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W18" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X18" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y18" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z18" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA18" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB18" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC18" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD18" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE18" s="4">
         <f t="shared" si="22"/>
@@ -2296,7 +2309,7 @@
     </row>
     <row r="19" spans="1:32" hidden="1">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="7">
         <v>42015</v>
@@ -2323,7 +2336,7 @@
       </c>
       <c r="H19" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I19" s="17">
         <f t="shared" si="20"/>
@@ -2331,87 +2344,87 @@
       </c>
       <c r="J19" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K19" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L19" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M19" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N19" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O19" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P19" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q19" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R19" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S19" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T19" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U19" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V19" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W19" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X19" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y19" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z19" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA19" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB19" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC19" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T19" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U19" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V19" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W19" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X19" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y19" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z19" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA19" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB19" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC19" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD19" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE19" s="4">
         <f t="shared" si="22"/>
@@ -2424,7 +2437,7 @@
     </row>
     <row r="20" spans="1:32" hidden="1">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="7">
         <v>42014</v>
@@ -2451,7 +2464,7 @@
       </c>
       <c r="H20" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I20" s="17">
         <f t="shared" si="20"/>
@@ -2459,87 +2472,87 @@
       </c>
       <c r="J20" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K20" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L20" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M20" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N20" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O20" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P20" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q20" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R20" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S20" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T20" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U20" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V20" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W20" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X20" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y20" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z20" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA20" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB20" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC20" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T20" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U20" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V20" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W20" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X20" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y20" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z20" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA20" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB20" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC20" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD20" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE20" s="4">
         <f t="shared" si="22"/>
@@ -2552,7 +2565,7 @@
     </row>
     <row r="21" spans="1:32" hidden="1">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="7">
         <v>42013</v>
@@ -2579,7 +2592,7 @@
       </c>
       <c r="H21" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I21" s="17">
         <f t="shared" si="20"/>
@@ -2587,87 +2600,87 @@
       </c>
       <c r="J21" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K21" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L21" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M21" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N21" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O21" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P21" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q21" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R21" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S21" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T21" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U21" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V21" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W21" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X21" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y21" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z21" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA21" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB21" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC21" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T21" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U21" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V21" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W21" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X21" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y21" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z21" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA21" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB21" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC21" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD21" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" si="22"/>
@@ -2680,7 +2693,7 @@
     </row>
     <row r="22" spans="1:32" hidden="1">
       <c r="A22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7">
         <v>42012</v>
@@ -2707,7 +2720,7 @@
       </c>
       <c r="H22" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I22" s="17">
         <f t="shared" si="20"/>
@@ -2715,87 +2728,87 @@
       </c>
       <c r="J22" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K22" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L22" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M22" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N22" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O22" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P22" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q22" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R22" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S22" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T22" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U22" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V22" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W22" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X22" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y22" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z22" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA22" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB22" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC22" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T22" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U22" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V22" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W22" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X22" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y22" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z22" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA22" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB22" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC22" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD22" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE22" s="4">
         <f t="shared" si="22"/>
@@ -2808,7 +2821,7 @@
     </row>
     <row r="23" spans="1:32" hidden="1">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7">
         <v>42011</v>
@@ -2835,7 +2848,7 @@
       </c>
       <c r="H23" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I23" s="17">
         <f t="shared" si="20"/>
@@ -2843,87 +2856,87 @@
       </c>
       <c r="J23" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K23" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L23" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M23" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N23" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O23" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P23" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q23" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R23" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S23" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T23" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U23" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V23" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W23" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X23" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y23" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z23" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA23" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB23" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC23" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T23" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U23" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V23" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W23" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X23" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y23" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z23" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA23" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB23" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC23" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD23" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE23" s="4">
         <f t="shared" si="22"/>
@@ -2936,7 +2949,7 @@
     </row>
     <row r="24" spans="1:32" hidden="1">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="7">
         <v>42010</v>
@@ -2963,7 +2976,7 @@
       </c>
       <c r="H24" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I24" s="17">
         <f t="shared" si="20"/>
@@ -2971,87 +2984,87 @@
       </c>
       <c r="J24" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K24" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L24" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M24" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N24" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O24" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P24" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q24" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R24" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S24" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T24" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U24" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V24" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W24" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X24" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y24" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z24" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA24" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB24" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC24" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T24" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U24" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V24" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W24" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X24" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y24" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z24" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA24" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB24" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC24" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD24" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE24" s="4">
         <f t="shared" si="22"/>
@@ -3064,7 +3077,7 @@
     </row>
     <row r="25" spans="1:32" hidden="1">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="7">
         <v>42009</v>
@@ -3091,7 +3104,7 @@
       </c>
       <c r="H25" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I25" s="17">
         <f t="shared" si="20"/>
@@ -3099,87 +3112,87 @@
       </c>
       <c r="J25" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K25" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L25" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M25" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N25" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O25" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P25" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q25" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R25" s="18">
         <f t="shared" si="20"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S25" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T25" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U25" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V25" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W25" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X25" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y25" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z25" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA25" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB25" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC25" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T25" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U25" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V25" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W25" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X25" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y25" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z25" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA25" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB25" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC25" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD25" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE25" s="4">
         <f t="shared" si="22"/>
@@ -3192,7 +3205,7 @@
     </row>
     <row r="26" spans="1:32" hidden="1">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="7">
         <v>42008</v>
@@ -3219,7 +3232,7 @@
       </c>
       <c r="H26" s="17">
         <f t="shared" si="20"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I26" s="17">
         <f t="shared" si="20"/>
@@ -3227,87 +3240,87 @@
       </c>
       <c r="J26" s="18">
         <f t="shared" si="20"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K26" s="16">
         <f t="shared" si="20"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L26" s="17">
         <f t="shared" si="20"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M26" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N26" s="18">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O26" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P26" s="17">
         <f t="shared" si="20"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q26" s="17">
         <f t="shared" si="20"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R26" s="18">
-        <f t="shared" ref="R26:W40" si="23">R27</f>
-        <v>4488</v>
+        <f t="shared" ref="R26:U39" si="23">R27</f>
+        <v>8516</v>
       </c>
       <c r="S26" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T26" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U26" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V26" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W26" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X26" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y26" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z26" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA26" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB26" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC26" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T26" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U26" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V26" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W26" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X26" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y26" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z26" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA26" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB26" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC26" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD26" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE26" s="4">
         <f t="shared" si="22"/>
@@ -3320,7 +3333,7 @@
     </row>
     <row r="27" spans="1:32" hidden="1">
       <c r="A27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B27" s="7">
         <v>42007</v>
@@ -3347,7 +3360,7 @@
       </c>
       <c r="H27" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I27" s="17">
         <f t="shared" si="24"/>
@@ -3355,87 +3368,87 @@
       </c>
       <c r="J27" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K27" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L27" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M27" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N27" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O27" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P27" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q27" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R27" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S27" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T27" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U27" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V27" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W27" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X27" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y27" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z27" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA27" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB27" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC27" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T27" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U27" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V27" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W27" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X27" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y27" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z27" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA27" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB27" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC27" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD27" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE27" s="4">
         <f t="shared" si="22"/>
@@ -3448,7 +3461,7 @@
     </row>
     <row r="28" spans="1:32" hidden="1">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="7">
         <v>42006</v>
@@ -3475,7 +3488,7 @@
       </c>
       <c r="H28" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I28" s="17">
         <f t="shared" si="24"/>
@@ -3483,87 +3496,87 @@
       </c>
       <c r="J28" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K28" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L28" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M28" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N28" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O28" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P28" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q28" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R28" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S28" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T28" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U28" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V28" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W28" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X28" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y28" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z28" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA28" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB28" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC28" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T28" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U28" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V28" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W28" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X28" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y28" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z28" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA28" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB28" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC28" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD28" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE28" s="4">
         <f t="shared" ref="AE28:AF44" si="25">SUM(C28,G28,K28,O28,S28,W28,AA28)-SUM(C29,G29,K29,O29,S29,W29,AA29)</f>
@@ -3576,7 +3589,7 @@
     </row>
     <row r="29" spans="1:32" hidden="1">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" s="7">
         <v>42005</v>
@@ -3603,7 +3616,7 @@
       </c>
       <c r="H29" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I29" s="17">
         <f t="shared" si="24"/>
@@ -3611,87 +3624,87 @@
       </c>
       <c r="J29" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K29" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L29" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M29" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O29" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P29" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q29" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R29" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S29" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T29" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U29" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V29" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W29" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X29" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y29" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z29" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA29" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB29" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC29" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T29" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U29" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V29" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W29" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X29" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y29" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z29" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA29" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB29" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC29" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD29" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE29" s="4">
         <f t="shared" si="25"/>
@@ -3704,7 +3717,7 @@
     </row>
     <row r="30" spans="1:32" hidden="1">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" s="7">
         <v>42004</v>
@@ -3731,7 +3744,7 @@
       </c>
       <c r="H30" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I30" s="17">
         <f t="shared" si="24"/>
@@ -3739,87 +3752,87 @@
       </c>
       <c r="J30" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K30" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L30" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M30" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N30" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O30" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P30" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q30" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R30" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S30" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T30" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U30" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V30" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W30" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X30" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y30" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z30" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA30" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB30" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC30" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T30" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U30" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V30" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W30" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X30" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y30" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z30" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA30" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB30" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC30" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD30" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE30" s="4">
         <f t="shared" si="25"/>
@@ -3832,7 +3845,7 @@
     </row>
     <row r="31" spans="1:32" hidden="1">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" s="7">
         <v>42003</v>
@@ -3859,7 +3872,7 @@
       </c>
       <c r="H31" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I31" s="17">
         <f t="shared" si="24"/>
@@ -3867,87 +3880,87 @@
       </c>
       <c r="J31" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K31" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L31" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M31" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N31" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O31" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P31" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q31" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R31" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S31" s="16">
         <f t="shared" si="21"/>
+        <v>12</v>
+      </c>
+      <c r="T31" s="17">
+        <f t="shared" si="21"/>
+        <v>7991</v>
+      </c>
+      <c r="U31" s="17">
+        <f t="shared" si="21"/>
+        <v>9</v>
+      </c>
+      <c r="V31" s="18">
+        <f t="shared" si="21"/>
+        <v>6258</v>
+      </c>
+      <c r="W31" s="16">
+        <f t="shared" si="21"/>
+        <v>27</v>
+      </c>
+      <c r="X31" s="17">
+        <f t="shared" si="21"/>
+        <v>28599</v>
+      </c>
+      <c r="Y31" s="17">
+        <f t="shared" si="21"/>
+        <v>4</v>
+      </c>
+      <c r="Z31" s="18">
+        <f t="shared" si="21"/>
+        <v>5367</v>
+      </c>
+      <c r="AA31" s="16">
+        <f t="shared" si="21"/>
+        <v>29</v>
+      </c>
+      <c r="AB31" s="17">
+        <f t="shared" si="21"/>
+        <v>48210</v>
+      </c>
+      <c r="AC31" s="17">
+        <f t="shared" si="21"/>
         <v>7</v>
       </c>
-      <c r="T31" s="17">
-        <f t="shared" si="21"/>
-        <v>3301</v>
-      </c>
-      <c r="U31" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="V31" s="18">
-        <f t="shared" si="21"/>
-        <v>1568</v>
-      </c>
-      <c r="W31" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="X31" s="17">
-        <f t="shared" si="21"/>
-        <v>27327</v>
-      </c>
-      <c r="Y31" s="17">
-        <f t="shared" si="21"/>
-        <v>4</v>
-      </c>
-      <c r="Z31" s="18">
-        <f t="shared" si="21"/>
-        <v>4095</v>
-      </c>
-      <c r="AA31" s="16">
-        <f t="shared" si="21"/>
-        <v>27</v>
-      </c>
-      <c r="AB31" s="17">
-        <f t="shared" si="21"/>
-        <v>42737</v>
-      </c>
-      <c r="AC31" s="17">
-        <f t="shared" si="21"/>
-        <v>5</v>
-      </c>
       <c r="AD31" s="18">
         <f t="shared" si="21"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE31" s="4">
         <f t="shared" si="25"/>
@@ -3960,7 +3973,7 @@
     </row>
     <row r="32" spans="1:32" hidden="1">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" s="7">
         <v>42002</v>
@@ -3987,7 +4000,7 @@
       </c>
       <c r="H32" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I32" s="17">
         <f t="shared" si="24"/>
@@ -3995,55 +4008,55 @@
       </c>
       <c r="J32" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K32" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L32" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M32" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N32" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O32" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P32" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q32" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R32" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S32" s="16">
         <f t="shared" si="21"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T32" s="17">
         <f t="shared" si="21"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U32" s="17">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V32" s="18">
         <f t="shared" ref="V32:AD39" si="26">V33</f>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W32" s="16">
         <f t="shared" si="26"/>
@@ -4051,7 +4064,7 @@
       </c>
       <c r="X32" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y32" s="17">
         <f t="shared" si="26"/>
@@ -4059,23 +4072,23 @@
       </c>
       <c r="Z32" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA32" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB32" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC32" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD32" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE32" s="4">
         <f t="shared" si="25"/>
@@ -4086,9 +4099,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:32" hidden="1">
+    <row r="33" spans="1:34" hidden="1">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="7">
         <v>42001</v>
@@ -4115,7 +4128,7 @@
       </c>
       <c r="H33" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I33" s="17">
         <f t="shared" si="24"/>
@@ -4123,55 +4136,55 @@
       </c>
       <c r="J33" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K33" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L33" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M33" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N33" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O33" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P33" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q33" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R33" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S33" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T33" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U33" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V33" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W33" s="16">
         <f t="shared" si="26"/>
@@ -4179,7 +4192,7 @@
       </c>
       <c r="X33" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y33" s="17">
         <f t="shared" si="26"/>
@@ -4187,23 +4200,23 @@
       </c>
       <c r="Z33" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA33" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB33" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC33" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD33" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE33" s="4">
         <f t="shared" si="25"/>
@@ -4214,9 +4227,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:32" hidden="1">
+    <row r="34" spans="1:34" hidden="1">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B34" s="7">
         <v>42000</v>
@@ -4243,7 +4256,7 @@
       </c>
       <c r="H34" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I34" s="17">
         <f t="shared" si="24"/>
@@ -4251,55 +4264,55 @@
       </c>
       <c r="J34" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K34" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L34" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M34" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N34" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O34" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P34" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q34" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R34" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S34" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T34" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U34" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V34" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W34" s="16">
         <f t="shared" si="26"/>
@@ -4307,7 +4320,7 @@
       </c>
       <c r="X34" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y34" s="17">
         <f t="shared" si="26"/>
@@ -4315,23 +4328,23 @@
       </c>
       <c r="Z34" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA34" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB34" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC34" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD34" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE34" s="4">
         <f t="shared" si="25"/>
@@ -4342,9 +4355,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:32" hidden="1">
+    <row r="35" spans="1:34" hidden="1">
       <c r="A35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="7">
         <v>41999</v>
@@ -4371,7 +4384,7 @@
       </c>
       <c r="H35" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I35" s="17">
         <f t="shared" si="24"/>
@@ -4379,55 +4392,55 @@
       </c>
       <c r="J35" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K35" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L35" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M35" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N35" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O35" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P35" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q35" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R35" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S35" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T35" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U35" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V35" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W35" s="16">
         <f t="shared" si="26"/>
@@ -4435,7 +4448,7 @@
       </c>
       <c r="X35" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y35" s="17">
         <f t="shared" si="26"/>
@@ -4443,23 +4456,23 @@
       </c>
       <c r="Z35" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA35" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB35" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC35" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD35" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE35" s="4">
         <f t="shared" si="25"/>
@@ -4470,9 +4483,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:32" hidden="1">
+    <row r="36" spans="1:34" hidden="1">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36" s="7">
         <v>41998</v>
@@ -4499,7 +4512,7 @@
       </c>
       <c r="H36" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I36" s="17">
         <f t="shared" si="24"/>
@@ -4507,55 +4520,55 @@
       </c>
       <c r="J36" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K36" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L36" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M36" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N36" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O36" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P36" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q36" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R36" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S36" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T36" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U36" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V36" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W36" s="16">
         <f t="shared" si="26"/>
@@ -4563,7 +4576,7 @@
       </c>
       <c r="X36" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y36" s="17">
         <f t="shared" si="26"/>
@@ -4571,23 +4584,23 @@
       </c>
       <c r="Z36" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA36" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB36" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC36" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD36" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE36" s="4">
         <f t="shared" si="25"/>
@@ -4598,9 +4611,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:32" hidden="1">
+    <row r="37" spans="1:34" hidden="1">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37" s="7">
         <v>41997</v>
@@ -4627,7 +4640,7 @@
       </c>
       <c r="H37" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I37" s="17">
         <f t="shared" si="24"/>
@@ -4635,55 +4648,55 @@
       </c>
       <c r="J37" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K37" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L37" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M37" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N37" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O37" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P37" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q37" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R37" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S37" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T37" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U37" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V37" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W37" s="16">
         <f t="shared" si="26"/>
@@ -4691,7 +4704,7 @@
       </c>
       <c r="X37" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y37" s="17">
         <f t="shared" si="26"/>
@@ -4699,23 +4712,23 @@
       </c>
       <c r="Z37" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA37" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB37" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC37" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD37" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE37" s="4">
         <f t="shared" si="25"/>
@@ -4726,9 +4739,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:32" hidden="1">
+    <row r="38" spans="1:34" hidden="1">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38" s="7">
         <v>41996</v>
@@ -4755,7 +4768,7 @@
       </c>
       <c r="H38" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I38" s="17">
         <f t="shared" si="24"/>
@@ -4763,55 +4776,55 @@
       </c>
       <c r="J38" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K38" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L38" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M38" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N38" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O38" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P38" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q38" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R38" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S38" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T38" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U38" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V38" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W38" s="16">
         <f t="shared" si="26"/>
@@ -4819,7 +4832,7 @@
       </c>
       <c r="X38" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y38" s="17">
         <f t="shared" si="26"/>
@@ -4827,23 +4840,23 @@
       </c>
       <c r="Z38" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA38" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB38" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC38" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD38" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE38" s="4">
         <f t="shared" si="25"/>
@@ -4854,9 +4867,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:32" hidden="1">
+    <row r="39" spans="1:34" hidden="1">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" s="7">
         <v>41995</v>
@@ -4883,7 +4896,7 @@
       </c>
       <c r="H39" s="17">
         <f t="shared" si="24"/>
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I39" s="17">
         <f t="shared" si="24"/>
@@ -4891,55 +4904,55 @@
       </c>
       <c r="J39" s="18">
         <f t="shared" si="24"/>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K39" s="16">
         <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L39" s="17">
         <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M39" s="17">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N39" s="18">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O39" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P39" s="17">
         <f t="shared" si="24"/>
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q39" s="17">
         <f t="shared" si="24"/>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R39" s="18">
         <f t="shared" si="23"/>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S39" s="16">
         <f t="shared" si="23"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T39" s="17">
         <f t="shared" si="23"/>
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U39" s="17">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V39" s="18">
         <f t="shared" si="26"/>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W39" s="16">
         <f t="shared" si="26"/>
@@ -4947,7 +4960,7 @@
       </c>
       <c r="X39" s="17">
         <f t="shared" si="26"/>
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y39" s="17">
         <f t="shared" si="26"/>
@@ -4955,23 +4968,23 @@
       </c>
       <c r="Z39" s="18">
         <f t="shared" si="26"/>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA39" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB39" s="17">
         <f t="shared" si="26"/>
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC39" s="17">
         <f t="shared" si="26"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD39" s="18">
         <f t="shared" si="26"/>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE39" s="4">
         <f t="shared" si="25"/>
@@ -4982,9 +4995,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:32">
+    <row r="40" spans="1:34">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40" s="7">
         <v>41994</v>
@@ -5008,7 +5021,7 @@
         <v>4</v>
       </c>
       <c r="H40" s="17">
-        <v>11700</v>
+        <v>11786</v>
       </c>
       <c r="I40" s="17">
         <f>G40-G41</f>
@@ -5016,57 +5029,55 @@
       </c>
       <c r="J40" s="18">
         <f>H40-H41</f>
-        <v>388</v>
+        <v>474</v>
       </c>
       <c r="K40" s="16">
-        <f t="shared" si="24"/>
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="L40" s="17">
-        <f t="shared" si="24"/>
-        <v>31855</v>
+        <v>38863</v>
       </c>
       <c r="M40" s="17">
         <f>K40-K41</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N40" s="18">
         <f>L40-L41</f>
-        <v>0</v>
+        <v>7008</v>
       </c>
       <c r="O40" s="16">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="P40" s="17">
-        <v>27212</v>
+        <v>31240</v>
       </c>
       <c r="Q40" s="17">
         <f>O40-O41</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="R40" s="18">
         <f>P40-P41</f>
-        <v>4488</v>
+        <v>8516</v>
       </c>
       <c r="S40" s="16">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="T40" s="17">
-        <v>3301</v>
+        <v>7991</v>
       </c>
       <c r="U40" s="17">
         <f>S40-S41</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="V40" s="18">
         <f>T40-T41</f>
-        <v>1568</v>
+        <v>6258</v>
       </c>
       <c r="W40" s="16">
         <v>27</v>
       </c>
       <c r="X40" s="17">
-        <v>27327</v>
+        <v>28599</v>
       </c>
       <c r="Y40" s="17">
         <f>W40-W41</f>
@@ -5074,34 +5085,41 @@
       </c>
       <c r="Z40" s="18">
         <f>X40-X41</f>
-        <v>4095</v>
+        <v>5367</v>
       </c>
       <c r="AA40" s="16">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AB40" s="17">
-        <v>42737</v>
+        <v>48210</v>
       </c>
       <c r="AC40" s="17">
         <f>AA40-AA41</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AD40" s="18">
         <f>AB40-AB41</f>
-        <v>2917</v>
+        <v>8390</v>
       </c>
       <c r="AE40" s="4">
         <f t="shared" si="25"/>
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="AF40" s="4">
         <f t="shared" si="25"/>
-        <v>18018</v>
+        <v>40575</v>
+      </c>
+      <c r="AG40">
+        <v>16477</v>
+      </c>
+      <c r="AH40">
+        <f>AG40-AG41</f>
+        <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:32">
+    <row r="41" spans="1:34">
       <c r="A41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" s="7">
         <v>41993</v>
@@ -5212,10 +5230,13 @@
         <f t="shared" si="25"/>
         <v>73206</v>
       </c>
+      <c r="AG41">
+        <v>16449</v>
+      </c>
     </row>
-    <row r="42" spans="1:32">
+    <row r="42" spans="1:34">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42" s="7">
         <v>41992</v>
@@ -5329,9 +5350,9 @@
         <v>20059</v>
       </c>
     </row>
-    <row r="43" spans="1:32">
+    <row r="43" spans="1:34">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B43" s="7">
         <v>41991</v>
@@ -5446,9 +5467,9 @@
         <v>18859</v>
       </c>
     </row>
-    <row r="44" spans="1:32">
+    <row r="44" spans="1:34">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B44" s="7">
         <v>41990</v>
@@ -5560,9 +5581,9 @@
         <v>20741</v>
       </c>
     </row>
-    <row r="45" spans="1:32">
+    <row r="45" spans="1:34">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B45" s="7">
         <v>41989</v>

</xml_diff>

<commit_message>
maj. Jeu de 22h à 23h
</commit_message>
<xml_diff>
--- a/mission wz.xlsx
+++ b/mission wz.xlsx
@@ -304,10 +304,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG42" sqref="AG42"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -718,61 +718,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37">
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19" t="s">
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19" t="s">
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19" t="s">
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
       <c r="AE1" t="s">
         <v>19</v>
       </c>
       <c r="AI1" s="1">
         <f ca="1">TODAY()</f>
-        <v>41994</v>
+        <v>41995</v>
       </c>
       <c r="AJ1" s="1">
         <v>42023</v>
       </c>
       <c r="AK1">
         <f ca="1">AJ1-AI1-1</f>
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -781,11 +781,11 @@
       </c>
       <c r="C2" s="8">
         <f>(150-C6)/150</f>
-        <v>0.26666666666666666</v>
+        <v>0.31333333333333335</v>
       </c>
       <c r="D2" s="8">
         <f>(150000-D6)/150000</f>
-        <v>0.18328</v>
+        <v>0.20276666666666668</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -811,11 +811,11 @@
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f t="shared" ref="O2" si="4">(150-O6)/150</f>
-        <v>0.29333333333333333</v>
+        <v>0.31333333333333335</v>
       </c>
       <c r="P2" s="8">
         <f t="shared" ref="P2" si="5">(150000-P6)/150000</f>
-        <v>0.20826666666666666</v>
+        <v>0.21629333333333334</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
@@ -831,21 +831,21 @@
       <c r="V2" s="8"/>
       <c r="W2" s="8">
         <f t="shared" ref="W2" si="8">(150-W6)/150</f>
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="X2" s="8">
         <f t="shared" ref="X2" si="9">(150000-X6)/150000</f>
-        <v>0.19066</v>
+        <v>0.20891999999999999</v>
       </c>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8">
         <f t="shared" ref="AA2" si="10">(150-AA6)/150</f>
-        <v>0.19333333333333333</v>
+        <v>0.2</v>
       </c>
       <c r="AB2" s="8">
         <f t="shared" ref="AB2" si="11">(150000-AB6)/150000</f>
-        <v>0.32140000000000002</v>
+        <v>0.32849333333333336</v>
       </c>
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
@@ -870,7 +870,7 @@
       </c>
       <c r="D3" s="9">
         <f ca="1">INT(D6/$AK$1)</f>
-        <v>4375</v>
+        <v>4429</v>
       </c>
       <c r="G3" s="9">
         <f ca="1">INT(G6/$AK$1)</f>
@@ -878,7 +878,7 @@
       </c>
       <c r="H3" s="9">
         <f ca="1">INT(H6/$AK$1)</f>
-        <v>4936</v>
+        <v>5119</v>
       </c>
       <c r="K3" s="9">
         <f ca="1">INT(K6/$AK$1)</f>
@@ -886,7 +886,7 @@
       </c>
       <c r="L3" s="9">
         <f ca="1">INT(L6/$AK$1)</f>
-        <v>3969</v>
+        <v>4116</v>
       </c>
       <c r="O3" s="9">
         <f ca="1">INT(O6/$AK$1)</f>
@@ -894,15 +894,15 @@
       </c>
       <c r="P3" s="9">
         <f ca="1">INT(P6/$AK$1)</f>
-        <v>4241</v>
+        <v>4353</v>
       </c>
       <c r="S3" s="9">
         <f ca="1">INT(S6/$AK$1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T3" s="9">
         <f ca="1">INT(T6/$AK$1)</f>
-        <v>5071</v>
+        <v>5259</v>
       </c>
       <c r="W3" s="9">
         <f ca="1">INT(W6/$AK$1)</f>
@@ -910,7 +910,7 @@
       </c>
       <c r="X3" s="9">
         <f ca="1">INT(X6/$AK$1)</f>
-        <v>4335</v>
+        <v>4394</v>
       </c>
       <c r="AA3" s="9">
         <f ca="1">INT(AA6/$AK$1)</f>
@@ -918,15 +918,15 @@
       </c>
       <c r="AB3" s="9">
         <f ca="1">INT(AB6/$AK$1)</f>
-        <v>3635</v>
+        <v>3730</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE4" ca="1" si="12">SUM(C3,G3,K3,O3,S3,W3,AA3)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AF3" s="5">
         <f ca="1">SUM(D3,H3,L3,P3,T3,X3,AB3)</f>
-        <v>30562</v>
+        <v>31400</v>
       </c>
       <c r="AI3" s="1">
         <v>41996</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="AK3" s="2">
         <f ca="1">(AK2-AK1)/AK2</f>
-        <v>0.15151515151515152</v>
+        <v>0.18181818181818182</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -1014,75 +1014,75 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-C6</f>
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-D6</f>
-        <v>1022</v>
+        <v>-467</v>
       </c>
       <c r="G5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-G6</f>
-        <v>-22</v>
+        <v>-26</v>
       </c>
       <c r="H5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-H6</f>
-        <v>-14684</v>
+        <v>-19096</v>
       </c>
       <c r="K5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-K6</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-L6</f>
-        <v>12393</v>
+        <v>7981</v>
       </c>
       <c r="O5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-O6</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-P6</f>
-        <v>4770</v>
+        <v>1562</v>
       </c>
       <c r="S5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-S6</f>
-        <v>-14</v>
+        <v>-18</v>
       </c>
       <c r="T5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-T6</f>
-        <v>-18479</v>
+        <v>-22891</v>
       </c>
       <c r="W5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-W6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-X6</f>
-        <v>2129</v>
+        <v>456</v>
       </c>
       <c r="AA5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-AA6</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-AB6</f>
-        <v>21740</v>
+        <v>18392</v>
       </c>
       <c r="AE5" s="5">
         <f ca="1">SUM(C5,G5,K5,O5,S5,W5,AA5)</f>
-        <v>12</v>
+        <v>-2</v>
       </c>
       <c r="AF5" s="5">
         <f ca="1">SUM(D5,H5,L5,P5,T5,X5,AB5)</f>
-        <v>8891</v>
+        <v>-14063</v>
       </c>
       <c r="AG5" s="3">
         <f ca="1">-$AK$3+AG6</f>
-        <v>3.3246753246753247E-2</v>
+        <v>1.6277056277056279E-2</v>
       </c>
       <c r="AH5" s="3">
         <f ca="1">AH6-$AK$3</f>
-        <v>3.3419134199134198E-2</v>
+        <v>1.0668484848484844E-2</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -1091,11 +1091,11 @@
       </c>
       <c r="C6" s="9">
         <f>150-C11</f>
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D6" s="9">
         <f>150000-D11</f>
-        <v>122508</v>
+        <v>119585</v>
       </c>
       <c r="G6" s="9">
         <f t="shared" ref="G6" si="14">150-G11</f>
@@ -1115,11 +1115,11 @@
       </c>
       <c r="O6" s="9">
         <f t="shared" ref="O6" si="16">150-O11</f>
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="P6" s="9">
         <f>150000-P11</f>
-        <v>118760</v>
+        <v>117556</v>
       </c>
       <c r="S6" s="9">
         <f t="shared" ref="S6" si="17">150-S11</f>
@@ -1131,35 +1131,35 @@
       </c>
       <c r="W6" s="9">
         <f t="shared" ref="W6" si="18">150-W11</f>
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="X6" s="9">
         <f>150000-X11</f>
-        <v>121401</v>
+        <v>118662</v>
       </c>
       <c r="AA6" s="9">
         <f t="shared" ref="AA6" si="19">150-AA11</f>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB6" s="9">
         <f>150000-AB11</f>
-        <v>101790</v>
+        <v>100726</v>
       </c>
       <c r="AE6" s="5">
         <f>SUM(C6,G6,K6,O6,S6,W6,AA6)</f>
-        <v>856</v>
+        <v>842</v>
       </c>
       <c r="AF6" s="5">
         <f>SUM(D6,H6,L6,P6,T6,X6,AB6)</f>
-        <v>855819</v>
+        <v>847889</v>
       </c>
       <c r="AG6" s="3">
         <f>(7*150-AE6)/(7*150)</f>
-        <v>0.18476190476190477</v>
+        <v>0.1980952380952381</v>
       </c>
       <c r="AH6" s="3">
         <f>(7*150000-AF6)/(7*150000)</f>
-        <v>0.18493428571428572</v>
+        <v>0.19248666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -1168,11 +1168,11 @@
       </c>
       <c r="AE7" s="5">
         <f>150*7-AE6</f>
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="AF7" s="5">
         <f>150000*7-AF6</f>
-        <v>194181</v>
+        <v>202111</v>
       </c>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
@@ -1276,10 +1276,10 @@
       <c r="AF10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="AG10" s="20" t="s">
+      <c r="AG10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="AH10" s="20" t="s">
+      <c r="AH10" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1292,11 +1292,11 @@
       </c>
       <c r="C11" s="13">
         <f t="shared" ref="C11:R26" si="20">C12</f>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D11" s="14">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E11" s="14">
         <f t="shared" si="20"/>
@@ -1340,11 +1340,11 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="20"/>
@@ -1372,11 +1372,11 @@
       </c>
       <c r="W11" s="13">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X11" s="14">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y11" s="14">
         <f t="shared" si="21"/>
@@ -1388,11 +1388,11 @@
       </c>
       <c r="AA11" s="13">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB11" s="14">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC11" s="14">
         <f t="shared" si="21"/>
@@ -1420,11 +1420,11 @@
       </c>
       <c r="C12" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D12" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E12" s="17">
         <f t="shared" si="20"/>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="O12" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P12" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q12" s="17">
         <f t="shared" si="20"/>
@@ -1500,11 +1500,11 @@
       </c>
       <c r="W12" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X12" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y12" s="17">
         <f t="shared" si="21"/>
@@ -1516,11 +1516,11 @@
       </c>
       <c r="AA12" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB12" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC12" s="17">
         <f t="shared" si="21"/>
@@ -1548,11 +1548,11 @@
       </c>
       <c r="C13" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D13" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E13" s="17">
         <f t="shared" si="20"/>
@@ -1596,11 +1596,11 @@
       </c>
       <c r="O13" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P13" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q13" s="17">
         <f t="shared" si="20"/>
@@ -1628,11 +1628,11 @@
       </c>
       <c r="W13" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X13" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y13" s="17">
         <f t="shared" si="21"/>
@@ -1644,11 +1644,11 @@
       </c>
       <c r="AA13" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB13" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC13" s="17">
         <f t="shared" si="21"/>
@@ -1676,11 +1676,11 @@
       </c>
       <c r="C14" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D14" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E14" s="17">
         <f t="shared" si="20"/>
@@ -1724,11 +1724,11 @@
       </c>
       <c r="O14" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P14" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q14" s="17">
         <f t="shared" si="20"/>
@@ -1756,11 +1756,11 @@
       </c>
       <c r="W14" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X14" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y14" s="17">
         <f t="shared" si="21"/>
@@ -1772,11 +1772,11 @@
       </c>
       <c r="AA14" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB14" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC14" s="17">
         <f t="shared" si="21"/>
@@ -1804,11 +1804,11 @@
       </c>
       <c r="C15" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D15" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E15" s="17">
         <f t="shared" si="20"/>
@@ -1852,11 +1852,11 @@
       </c>
       <c r="O15" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P15" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q15" s="17">
         <f t="shared" si="20"/>
@@ -1884,11 +1884,11 @@
       </c>
       <c r="W15" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X15" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y15" s="17">
         <f t="shared" si="21"/>
@@ -1900,11 +1900,11 @@
       </c>
       <c r="AA15" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB15" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC15" s="17">
         <f t="shared" si="21"/>
@@ -1932,11 +1932,11 @@
       </c>
       <c r="C16" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D16" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E16" s="17">
         <f t="shared" si="20"/>
@@ -1980,11 +1980,11 @@
       </c>
       <c r="O16" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P16" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q16" s="17">
         <f t="shared" si="20"/>
@@ -2012,11 +2012,11 @@
       </c>
       <c r="W16" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X16" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y16" s="17">
         <f t="shared" si="21"/>
@@ -2028,11 +2028,11 @@
       </c>
       <c r="AA16" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB16" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC16" s="17">
         <f t="shared" si="21"/>
@@ -2060,11 +2060,11 @@
       </c>
       <c r="C17" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D17" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E17" s="17">
         <f t="shared" si="20"/>
@@ -2108,11 +2108,11 @@
       </c>
       <c r="O17" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P17" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q17" s="17">
         <f t="shared" si="20"/>
@@ -2140,11 +2140,11 @@
       </c>
       <c r="W17" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X17" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y17" s="17">
         <f t="shared" si="21"/>
@@ -2156,11 +2156,11 @@
       </c>
       <c r="AA17" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB17" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC17" s="17">
         <f t="shared" si="21"/>
@@ -2188,11 +2188,11 @@
       </c>
       <c r="C18" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D18" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E18" s="17">
         <f t="shared" si="20"/>
@@ -2236,11 +2236,11 @@
       </c>
       <c r="O18" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P18" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q18" s="17">
         <f t="shared" si="20"/>
@@ -2268,11 +2268,11 @@
       </c>
       <c r="W18" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X18" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y18" s="17">
         <f t="shared" si="21"/>
@@ -2284,11 +2284,11 @@
       </c>
       <c r="AA18" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB18" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC18" s="17">
         <f t="shared" si="21"/>
@@ -2316,11 +2316,11 @@
       </c>
       <c r="C19" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D19" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E19" s="17">
         <f t="shared" si="20"/>
@@ -2364,11 +2364,11 @@
       </c>
       <c r="O19" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P19" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q19" s="17">
         <f t="shared" si="20"/>
@@ -2396,11 +2396,11 @@
       </c>
       <c r="W19" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X19" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y19" s="17">
         <f t="shared" si="21"/>
@@ -2412,11 +2412,11 @@
       </c>
       <c r="AA19" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB19" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC19" s="17">
         <f t="shared" si="21"/>
@@ -2444,11 +2444,11 @@
       </c>
       <c r="C20" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D20" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E20" s="17">
         <f t="shared" si="20"/>
@@ -2492,11 +2492,11 @@
       </c>
       <c r="O20" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P20" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q20" s="17">
         <f t="shared" si="20"/>
@@ -2524,11 +2524,11 @@
       </c>
       <c r="W20" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X20" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y20" s="17">
         <f t="shared" si="21"/>
@@ -2540,11 +2540,11 @@
       </c>
       <c r="AA20" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB20" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC20" s="17">
         <f t="shared" si="21"/>
@@ -2572,11 +2572,11 @@
       </c>
       <c r="C21" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D21" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E21" s="17">
         <f t="shared" si="20"/>
@@ -2620,11 +2620,11 @@
       </c>
       <c r="O21" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P21" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q21" s="17">
         <f t="shared" si="20"/>
@@ -2652,11 +2652,11 @@
       </c>
       <c r="W21" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X21" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y21" s="17">
         <f t="shared" si="21"/>
@@ -2668,11 +2668,11 @@
       </c>
       <c r="AA21" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB21" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC21" s="17">
         <f t="shared" si="21"/>
@@ -2700,11 +2700,11 @@
       </c>
       <c r="C22" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D22" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E22" s="17">
         <f t="shared" si="20"/>
@@ -2748,11 +2748,11 @@
       </c>
       <c r="O22" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P22" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q22" s="17">
         <f t="shared" si="20"/>
@@ -2780,11 +2780,11 @@
       </c>
       <c r="W22" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X22" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y22" s="17">
         <f t="shared" si="21"/>
@@ -2796,11 +2796,11 @@
       </c>
       <c r="AA22" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB22" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC22" s="17">
         <f t="shared" si="21"/>
@@ -2828,11 +2828,11 @@
       </c>
       <c r="C23" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D23" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E23" s="17">
         <f t="shared" si="20"/>
@@ -2876,11 +2876,11 @@
       </c>
       <c r="O23" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P23" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q23" s="17">
         <f t="shared" si="20"/>
@@ -2908,11 +2908,11 @@
       </c>
       <c r="W23" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X23" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y23" s="17">
         <f t="shared" si="21"/>
@@ -2924,11 +2924,11 @@
       </c>
       <c r="AA23" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB23" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC23" s="17">
         <f t="shared" si="21"/>
@@ -2956,11 +2956,11 @@
       </c>
       <c r="C24" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D24" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E24" s="17">
         <f t="shared" si="20"/>
@@ -3004,11 +3004,11 @@
       </c>
       <c r="O24" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P24" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q24" s="17">
         <f t="shared" si="20"/>
@@ -3036,11 +3036,11 @@
       </c>
       <c r="W24" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X24" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y24" s="17">
         <f t="shared" si="21"/>
@@ -3052,11 +3052,11 @@
       </c>
       <c r="AA24" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB24" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC24" s="17">
         <f t="shared" si="21"/>
@@ -3084,11 +3084,11 @@
       </c>
       <c r="C25" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D25" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E25" s="17">
         <f t="shared" si="20"/>
@@ -3132,11 +3132,11 @@
       </c>
       <c r="O25" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P25" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q25" s="17">
         <f t="shared" si="20"/>
@@ -3164,11 +3164,11 @@
       </c>
       <c r="W25" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X25" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y25" s="17">
         <f t="shared" si="21"/>
@@ -3180,11 +3180,11 @@
       </c>
       <c r="AA25" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB25" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC25" s="17">
         <f t="shared" si="21"/>
@@ -3212,11 +3212,11 @@
       </c>
       <c r="C26" s="16">
         <f t="shared" si="20"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D26" s="17">
         <f t="shared" si="20"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E26" s="17">
         <f t="shared" si="20"/>
@@ -3260,11 +3260,11 @@
       </c>
       <c r="O26" s="16">
         <f t="shared" si="20"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P26" s="17">
         <f t="shared" si="20"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q26" s="17">
         <f t="shared" si="20"/>
@@ -3292,11 +3292,11 @@
       </c>
       <c r="W26" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X26" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y26" s="17">
         <f t="shared" si="21"/>
@@ -3308,11 +3308,11 @@
       </c>
       <c r="AA26" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB26" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC26" s="17">
         <f t="shared" si="21"/>
@@ -3340,11 +3340,11 @@
       </c>
       <c r="C27" s="16">
         <f t="shared" ref="C27:Q40" si="24">C28</f>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D27" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E27" s="17">
         <f t="shared" si="24"/>
@@ -3388,11 +3388,11 @@
       </c>
       <c r="O27" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P27" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q27" s="17">
         <f t="shared" si="24"/>
@@ -3420,11 +3420,11 @@
       </c>
       <c r="W27" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X27" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y27" s="17">
         <f t="shared" si="21"/>
@@ -3436,11 +3436,11 @@
       </c>
       <c r="AA27" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB27" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC27" s="17">
         <f t="shared" si="21"/>
@@ -3468,11 +3468,11 @@
       </c>
       <c r="C28" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D28" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E28" s="17">
         <f t="shared" si="24"/>
@@ -3516,11 +3516,11 @@
       </c>
       <c r="O28" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P28" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q28" s="17">
         <f t="shared" si="24"/>
@@ -3548,11 +3548,11 @@
       </c>
       <c r="W28" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X28" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y28" s="17">
         <f t="shared" si="21"/>
@@ -3564,11 +3564,11 @@
       </c>
       <c r="AA28" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB28" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC28" s="17">
         <f t="shared" si="21"/>
@@ -3596,11 +3596,11 @@
       </c>
       <c r="C29" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D29" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E29" s="17">
         <f t="shared" si="24"/>
@@ -3644,11 +3644,11 @@
       </c>
       <c r="O29" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P29" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q29" s="17">
         <f t="shared" si="24"/>
@@ -3676,11 +3676,11 @@
       </c>
       <c r="W29" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X29" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y29" s="17">
         <f t="shared" si="21"/>
@@ -3692,11 +3692,11 @@
       </c>
       <c r="AA29" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB29" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC29" s="17">
         <f t="shared" si="21"/>
@@ -3724,11 +3724,11 @@
       </c>
       <c r="C30" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D30" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E30" s="17">
         <f t="shared" si="24"/>
@@ -3772,11 +3772,11 @@
       </c>
       <c r="O30" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P30" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q30" s="17">
         <f t="shared" si="24"/>
@@ -3804,11 +3804,11 @@
       </c>
       <c r="W30" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X30" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y30" s="17">
         <f t="shared" si="21"/>
@@ -3820,11 +3820,11 @@
       </c>
       <c r="AA30" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB30" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC30" s="17">
         <f t="shared" si="21"/>
@@ -3852,11 +3852,11 @@
       </c>
       <c r="C31" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D31" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E31" s="17">
         <f t="shared" si="24"/>
@@ -3900,11 +3900,11 @@
       </c>
       <c r="O31" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P31" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q31" s="17">
         <f t="shared" si="24"/>
@@ -3932,11 +3932,11 @@
       </c>
       <c r="W31" s="16">
         <f t="shared" si="21"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X31" s="17">
         <f t="shared" si="21"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y31" s="17">
         <f t="shared" si="21"/>
@@ -3948,11 +3948,11 @@
       </c>
       <c r="AA31" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB31" s="17">
         <f t="shared" si="21"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC31" s="17">
         <f t="shared" si="21"/>
@@ -3980,11 +3980,11 @@
       </c>
       <c r="C32" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D32" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E32" s="17">
         <f t="shared" si="24"/>
@@ -4028,11 +4028,11 @@
       </c>
       <c r="O32" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P32" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q32" s="17">
         <f t="shared" si="24"/>
@@ -4060,11 +4060,11 @@
       </c>
       <c r="W32" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X32" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y32" s="17">
         <f t="shared" si="26"/>
@@ -4076,11 +4076,11 @@
       </c>
       <c r="AA32" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB32" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC32" s="17">
         <f t="shared" si="26"/>
@@ -4108,11 +4108,11 @@
       </c>
       <c r="C33" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D33" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E33" s="17">
         <f t="shared" si="24"/>
@@ -4156,11 +4156,11 @@
       </c>
       <c r="O33" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P33" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q33" s="17">
         <f t="shared" si="24"/>
@@ -4188,11 +4188,11 @@
       </c>
       <c r="W33" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X33" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y33" s="17">
         <f t="shared" si="26"/>
@@ -4204,11 +4204,11 @@
       </c>
       <c r="AA33" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB33" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC33" s="17">
         <f t="shared" si="26"/>
@@ -4236,11 +4236,11 @@
       </c>
       <c r="C34" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D34" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E34" s="17">
         <f t="shared" si="24"/>
@@ -4284,11 +4284,11 @@
       </c>
       <c r="O34" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P34" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q34" s="17">
         <f t="shared" si="24"/>
@@ -4316,11 +4316,11 @@
       </c>
       <c r="W34" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X34" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y34" s="17">
         <f t="shared" si="26"/>
@@ -4332,11 +4332,11 @@
       </c>
       <c r="AA34" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB34" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC34" s="17">
         <f t="shared" si="26"/>
@@ -4364,11 +4364,11 @@
       </c>
       <c r="C35" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D35" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E35" s="17">
         <f t="shared" si="24"/>
@@ -4412,11 +4412,11 @@
       </c>
       <c r="O35" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P35" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q35" s="17">
         <f t="shared" si="24"/>
@@ -4444,11 +4444,11 @@
       </c>
       <c r="W35" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X35" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y35" s="17">
         <f t="shared" si="26"/>
@@ -4460,11 +4460,11 @@
       </c>
       <c r="AA35" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB35" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC35" s="17">
         <f t="shared" si="26"/>
@@ -4492,11 +4492,11 @@
       </c>
       <c r="C36" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D36" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E36" s="17">
         <f t="shared" si="24"/>
@@ -4540,11 +4540,11 @@
       </c>
       <c r="O36" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P36" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q36" s="17">
         <f t="shared" si="24"/>
@@ -4572,11 +4572,11 @@
       </c>
       <c r="W36" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X36" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y36" s="17">
         <f t="shared" si="26"/>
@@ -4588,11 +4588,11 @@
       </c>
       <c r="AA36" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB36" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC36" s="17">
         <f t="shared" si="26"/>
@@ -4620,11 +4620,11 @@
       </c>
       <c r="C37" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D37" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="24"/>
@@ -4668,11 +4668,11 @@
       </c>
       <c r="O37" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P37" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q37" s="17">
         <f t="shared" si="24"/>
@@ -4700,11 +4700,11 @@
       </c>
       <c r="W37" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X37" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y37" s="17">
         <f t="shared" si="26"/>
@@ -4716,11 +4716,11 @@
       </c>
       <c r="AA37" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB37" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC37" s="17">
         <f t="shared" si="26"/>
@@ -4748,11 +4748,11 @@
       </c>
       <c r="C38" s="16">
         <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D38" s="17">
         <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E38" s="17">
         <f t="shared" si="24"/>
@@ -4796,11 +4796,11 @@
       </c>
       <c r="O38" s="16">
         <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P38" s="17">
         <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q38" s="17">
         <f t="shared" si="24"/>
@@ -4828,11 +4828,11 @@
       </c>
       <c r="W38" s="16">
         <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X38" s="17">
         <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y38" s="17">
         <f t="shared" si="26"/>
@@ -4844,11 +4844,11 @@
       </c>
       <c r="AA38" s="16">
         <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB38" s="17">
         <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC38" s="17">
         <f t="shared" si="26"/>
@@ -4867,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:34" hidden="1">
+    <row r="39" spans="1:34">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -4875,12 +4875,10 @@
         <v>41995</v>
       </c>
       <c r="C39" s="16">
-        <f t="shared" si="24"/>
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D39" s="17">
-        <f t="shared" si="24"/>
-        <v>27492</v>
+        <v>30415</v>
       </c>
       <c r="E39" s="17">
         <f t="shared" si="24"/>
@@ -4923,12 +4921,10 @@
         <v>7008</v>
       </c>
       <c r="O39" s="16">
-        <f t="shared" si="24"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="P39" s="17">
-        <f t="shared" si="24"/>
-        <v>31240</v>
+        <v>32444</v>
       </c>
       <c r="Q39" s="17">
         <f t="shared" si="24"/>
@@ -4955,12 +4951,10 @@
         <v>6258</v>
       </c>
       <c r="W39" s="16">
-        <f t="shared" si="26"/>
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="X39" s="17">
-        <f t="shared" si="26"/>
-        <v>28599</v>
+        <v>31338</v>
       </c>
       <c r="Y39" s="17">
         <f t="shared" si="26"/>
@@ -4971,12 +4965,10 @@
         <v>5367</v>
       </c>
       <c r="AA39" s="16">
-        <f t="shared" si="26"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AB39" s="17">
-        <f t="shared" si="26"/>
-        <v>48210</v>
+        <v>49274</v>
       </c>
       <c r="AC39" s="17">
         <f t="shared" si="26"/>
@@ -4988,11 +4980,18 @@
       </c>
       <c r="AE39" s="4">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="AF39" s="4">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>7930</v>
+      </c>
+      <c r="AG39">
+        <v>16487</v>
+      </c>
+      <c r="AH39">
+        <f>AG39-AG40</f>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:34">

</xml_diff>

<commit_message>
début parti 19:30 23/12/2014
</commit_message>
<xml_diff>
--- a/mission wz.xlsx
+++ b/mission wz.xlsx
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -765,14 +765,14 @@
       </c>
       <c r="AI1" s="1">
         <f ca="1">TODAY()</f>
-        <v>41995</v>
+        <v>41996</v>
       </c>
       <c r="AJ1" s="1">
         <v>42023</v>
       </c>
       <c r="AK1">
         <f ca="1">AJ1-AI1-1</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -791,7 +791,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8">
         <f t="shared" ref="G2" si="0">(150-G6)/150</f>
-        <v>2.6666666666666668E-2</v>
+        <v>3.3333333333333333E-2</v>
       </c>
       <c r="H2" s="8">
         <f t="shared" ref="H2" si="1">(150000-H6)/150000</f>
@@ -870,7 +870,7 @@
       </c>
       <c r="D3" s="9">
         <f ca="1">INT(D6/$AK$1)</f>
-        <v>4429</v>
+        <v>4599</v>
       </c>
       <c r="G3" s="9">
         <f ca="1">INT(G6/$AK$1)</f>
@@ -878,7 +878,7 @@
       </c>
       <c r="H3" s="9">
         <f ca="1">INT(H6/$AK$1)</f>
-        <v>5119</v>
+        <v>5315</v>
       </c>
       <c r="K3" s="9">
         <f ca="1">INT(K6/$AK$1)</f>
@@ -886,7 +886,7 @@
       </c>
       <c r="L3" s="9">
         <f ca="1">INT(L6/$AK$1)</f>
-        <v>4116</v>
+        <v>4274</v>
       </c>
       <c r="O3" s="9">
         <f ca="1">INT(O6/$AK$1)</f>
@@ -894,7 +894,7 @@
       </c>
       <c r="P3" s="9">
         <f ca="1">INT(P6/$AK$1)</f>
-        <v>4353</v>
+        <v>4521</v>
       </c>
       <c r="S3" s="9">
         <f ca="1">INT(S6/$AK$1)</f>
@@ -902,7 +902,7 @@
       </c>
       <c r="T3" s="9">
         <f ca="1">INT(T6/$AK$1)</f>
-        <v>5259</v>
+        <v>5461</v>
       </c>
       <c r="W3" s="9">
         <f ca="1">INT(W6/$AK$1)</f>
@@ -910,7 +910,7 @@
       </c>
       <c r="X3" s="9">
         <f ca="1">INT(X6/$AK$1)</f>
-        <v>4394</v>
+        <v>4563</v>
       </c>
       <c r="AA3" s="9">
         <f ca="1">INT(AA6/$AK$1)</f>
@@ -918,7 +918,7 @@
       </c>
       <c r="AB3" s="9">
         <f ca="1">INT(AB6/$AK$1)</f>
-        <v>3730</v>
+        <v>3874</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE4" ca="1" si="12">SUM(C3,G3,K3,O3,S3,W3,AA3)</f>
@@ -926,7 +926,7 @@
       </c>
       <c r="AF3" s="5">
         <f ca="1">SUM(D3,H3,L3,P3,T3,X3,AB3)</f>
-        <v>31400</v>
+        <v>32607</v>
       </c>
       <c r="AI3" s="1">
         <v>41996</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="AK3" s="2">
         <f ca="1">(AK2-AK1)/AK2</f>
-        <v>0.18181818181818182</v>
+        <v>0.21212121212121213</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -1014,75 +1014,75 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-C6</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-D6</f>
-        <v>-467</v>
+        <v>-4879</v>
       </c>
       <c r="G5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-G6</f>
-        <v>-26</v>
+        <v>-30</v>
       </c>
       <c r="H5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-H6</f>
-        <v>-19096</v>
+        <v>-23508</v>
       </c>
       <c r="K5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-K6</f>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-L6</f>
-        <v>7981</v>
+        <v>3569</v>
       </c>
       <c r="O5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-O6</f>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="P5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-P6</f>
-        <v>1562</v>
+        <v>-2850</v>
       </c>
       <c r="S5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-S6</f>
-        <v>-18</v>
+        <v>-23</v>
       </c>
       <c r="T5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-T6</f>
-        <v>-22891</v>
+        <v>-27303</v>
       </c>
       <c r="W5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-W6</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="X5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-X6</f>
-        <v>456</v>
+        <v>-3956</v>
       </c>
       <c r="AA5" s="9">
         <f ca="1">150-INT(150-150/34*$AK$1)-AA6</f>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="AB5" s="9">
         <f ca="1">150000-INT(150000-150000/34*$AK$1)-AB6</f>
-        <v>18392</v>
+        <v>13980</v>
       </c>
       <c r="AE5" s="5">
         <f ca="1">SUM(C5,G5,K5,O5,S5,W5,AA5)</f>
-        <v>-2</v>
+        <v>-36</v>
       </c>
       <c r="AF5" s="5">
         <f ca="1">SUM(D5,H5,L5,P5,T5,X5,AB5)</f>
-        <v>-14063</v>
+        <v>-44947</v>
       </c>
       <c r="AG5" s="3">
         <f ca="1">-$AK$3+AG6</f>
-        <v>1.6277056277056279E-2</v>
+        <v>-1.3073593073593071E-2</v>
       </c>
       <c r="AH5" s="3">
         <f ca="1">AH6-$AK$3</f>
-        <v>1.0668484848484844E-2</v>
+        <v>-1.963454545454546E-2</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -1099,7 +1099,7 @@
       </c>
       <c r="G6" s="9">
         <f t="shared" ref="G6" si="14">150-G11</f>
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H6" s="9">
         <f>150000-H11</f>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="AE6" s="5">
         <f>SUM(C6,G6,K6,O6,S6,W6,AA6)</f>
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="AF6" s="5">
         <f>SUM(D6,H6,L6,P6,T6,X6,AB6)</f>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="AG6" s="3">
         <f>(7*150-AE6)/(7*150)</f>
-        <v>0.1980952380952381</v>
+        <v>0.19904761904761906</v>
       </c>
       <c r="AH6" s="3">
         <f>(7*150000-AF6)/(7*150000)</f>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="AE7" s="5">
         <f>150*7-AE6</f>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="AF7" s="5">
         <f>150000*7-AF6</f>
@@ -1308,7 +1308,7 @@
       </c>
       <c r="G11" s="13">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" s="14">
         <f t="shared" si="20"/>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="G12" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H12" s="17">
         <f t="shared" si="20"/>
@@ -1564,7 +1564,7 @@
       </c>
       <c r="G13" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H13" s="17">
         <f t="shared" si="20"/>
@@ -1692,7 +1692,7 @@
       </c>
       <c r="G14" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H14" s="17">
         <f t="shared" si="20"/>
@@ -1820,7 +1820,7 @@
       </c>
       <c r="G15" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H15" s="17">
         <f t="shared" si="20"/>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G16" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H16" s="17">
         <f t="shared" si="20"/>
@@ -2076,7 +2076,7 @@
       </c>
       <c r="G17" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H17" s="17">
         <f t="shared" si="20"/>
@@ -2204,7 +2204,7 @@
       </c>
       <c r="G18" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H18" s="17">
         <f t="shared" si="20"/>
@@ -2332,7 +2332,7 @@
       </c>
       <c r="G19" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H19" s="17">
         <f t="shared" si="20"/>
@@ -2460,7 +2460,7 @@
       </c>
       <c r="G20" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H20" s="17">
         <f t="shared" si="20"/>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="G21" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H21" s="17">
         <f t="shared" si="20"/>
@@ -2716,7 +2716,7 @@
       </c>
       <c r="G22" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22" s="17">
         <f t="shared" si="20"/>
@@ -2844,7 +2844,7 @@
       </c>
       <c r="G23" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H23" s="17">
         <f t="shared" si="20"/>
@@ -2972,7 +2972,7 @@
       </c>
       <c r="G24" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H24" s="17">
         <f t="shared" si="20"/>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="G25" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H25" s="17">
         <f t="shared" si="20"/>
@@ -3228,7 +3228,7 @@
       </c>
       <c r="G26" s="16">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H26" s="17">
         <f t="shared" si="20"/>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="G27" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H27" s="17">
         <f t="shared" si="24"/>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="G28" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H28" s="17">
         <f t="shared" si="24"/>
@@ -3612,7 +3612,7 @@
       </c>
       <c r="G29" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H29" s="17">
         <f t="shared" si="24"/>
@@ -3740,7 +3740,7 @@
       </c>
       <c r="G30" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H30" s="17">
         <f t="shared" si="24"/>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="G31" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H31" s="17">
         <f t="shared" si="24"/>
@@ -3996,7 +3996,7 @@
       </c>
       <c r="G32" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H32" s="17">
         <f t="shared" si="24"/>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="G33" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H33" s="17">
         <f t="shared" si="24"/>
@@ -4252,7 +4252,7 @@
       </c>
       <c r="G34" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H34" s="17">
         <f t="shared" si="24"/>
@@ -4380,7 +4380,7 @@
       </c>
       <c r="G35" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H35" s="17">
         <f t="shared" si="24"/>
@@ -4508,7 +4508,7 @@
       </c>
       <c r="G36" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H36" s="17">
         <f t="shared" si="24"/>
@@ -4636,7 +4636,7 @@
       </c>
       <c r="G37" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H37" s="17">
         <f t="shared" si="24"/>
@@ -4764,7 +4764,7 @@
       </c>
       <c r="G38" s="16">
         <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H38" s="17">
         <f t="shared" si="24"/>
@@ -4889,8 +4889,7 @@
         <v>4562</v>
       </c>
       <c r="G39" s="16">
-        <f t="shared" si="24"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H39" s="17">
         <f t="shared" si="24"/>
@@ -4980,7 +4979,7 @@
       </c>
       <c r="AE39" s="4">
         <f t="shared" si="25"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AF39" s="4">
         <f t="shared" si="25"/>

</xml_diff>

<commit_message>
maj - 22h30 à 01-47
</commit_message>
<xml_diff>
--- a/mission wz.xlsx
+++ b/mission wz.xlsx
@@ -668,7 +668,7 @@
   <dimension ref="A1:AK45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA37" sqref="AA37"/>
+      <selection activeCell="X36" sqref="X36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -754,14 +754,14 @@
       </c>
       <c r="AI1" s="1">
         <f ca="1">TODAY()</f>
-        <v>41998</v>
+        <v>41999</v>
       </c>
       <c r="AJ1" s="1">
         <v>42023</v>
       </c>
       <c r="AK1">
         <f ca="1">AJ1-AI1-1</f>
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:37">
@@ -770,71 +770,71 @@
       </c>
       <c r="C2" s="8">
         <f>(150-C6)/150</f>
-        <v>0.34</v>
+        <v>0.37333333333333335</v>
       </c>
       <c r="D2" s="8">
         <f>(150000-D6)/150000</f>
-        <v>0.24197333333333335</v>
+        <v>0.24800666666666665</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8">
         <f t="shared" ref="G2" si="0">(150-G6)/150</f>
-        <v>0.16666666666666666</v>
+        <v>0.22</v>
       </c>
       <c r="H2" s="8">
         <f t="shared" ref="H2" si="1">(150000-H6)/150000</f>
-        <v>0.22022666666666665</v>
+        <v>0.26561333333333331</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8">
         <f t="shared" ref="K2" si="2">(150-K6)/150</f>
-        <v>0.29333333333333333</v>
+        <v>0.32</v>
       </c>
       <c r="L2" s="8">
         <f t="shared" ref="L2" si="3">(150000-L6)/150000</f>
-        <v>0.32658666666666669</v>
+        <v>0.35833999999999999</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8">
         <f t="shared" ref="O2" si="4">(150-O6)/150</f>
-        <v>0.45333333333333331</v>
+        <v>0.46</v>
       </c>
       <c r="P2" s="8">
         <f t="shared" ref="P2" si="5">(150000-P6)/150000</f>
-        <v>0.31106</v>
+        <v>0.31427333333333335</v>
       </c>
       <c r="Q2" s="8"/>
       <c r="R2" s="8"/>
       <c r="S2" s="8">
         <f t="shared" ref="S2" si="6">(150-S6)/150</f>
-        <v>0.1</v>
+        <v>0.12666666666666668</v>
       </c>
       <c r="T2" s="8">
         <f t="shared" ref="T2" si="7">(150000-T6)/150000</f>
-        <v>6.3920000000000005E-2</v>
+        <v>7.5219999999999995E-2</v>
       </c>
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
       <c r="W2" s="8">
         <f t="shared" ref="W2" si="8">(150-W6)/150</f>
-        <v>0.32</v>
+        <v>0.32666666666666666</v>
       </c>
       <c r="X2" s="8">
         <f t="shared" ref="X2" si="9">(150000-X6)/150000</f>
-        <v>0.30562666666666666</v>
+        <v>0.308</v>
       </c>
       <c r="Y2" s="8"/>
       <c r="Z2" s="8"/>
       <c r="AA2" s="8">
         <f t="shared" ref="AA2" si="10">(150-AA6)/150</f>
-        <v>0.29333333333333333</v>
+        <v>0.30666666666666664</v>
       </c>
       <c r="AB2" s="8">
         <f t="shared" ref="AB2" si="11">(150000-AB6)/150000</f>
-        <v>0.37947999999999998</v>
+        <v>0.40846666666666664</v>
       </c>
       <c r="AC2" s="8"/>
       <c r="AD2" s="8"/>
@@ -859,7 +859,7 @@
       </c>
       <c r="D3" s="9">
         <f ca="1">IF(D6&lt;0,0,INT(D6/$AK$1))</f>
-        <v>4737</v>
+        <v>4904</v>
       </c>
       <c r="G3" s="9">
         <f ca="1">IF(G6&lt;0,0,INT(G6/$AK$1))</f>
@@ -867,7 +867,7 @@
       </c>
       <c r="H3" s="9">
         <f ca="1">IF(H6&lt;0,0,INT(H6/$AK$1))</f>
-        <v>4873</v>
+        <v>4789</v>
       </c>
       <c r="K3" s="9">
         <f ca="1">IF(K6&lt;0,0,INT(K6/$AK$1))</f>
@@ -875,7 +875,7 @@
       </c>
       <c r="L3" s="9">
         <f ca="1">IF(L6&lt;0,0,INT(L6/$AK$1))</f>
-        <v>4208</v>
+        <v>4184</v>
       </c>
       <c r="O3" s="9">
         <f ca="1">IF(O6&lt;0,0,INT(O6/$AK$1))</f>
@@ -883,7 +883,7 @@
       </c>
       <c r="P3" s="9">
         <f ca="1">IF(P6&lt;0,0,INT(P6/$AK$1))</f>
-        <v>4305</v>
+        <v>4472</v>
       </c>
       <c r="S3" s="9">
         <f ca="1">IF(S6&lt;0,0,INT(S6/$AK$1))</f>
@@ -891,7 +891,7 @@
       </c>
       <c r="T3" s="9">
         <f ca="1">IF(T6&lt;0,0,INT(T6/$AK$1))</f>
-        <v>5850</v>
+        <v>6031</v>
       </c>
       <c r="W3" s="9">
         <f ca="1">IF(W6&lt;0,0,INT(W6/$AK$1))</f>
@@ -899,7 +899,7 @@
       </c>
       <c r="X3" s="9">
         <f ca="1">IF(X6&lt;0,0,INT(X6/$AK$1))</f>
-        <v>4339</v>
+        <v>4513</v>
       </c>
       <c r="AA3" s="9">
         <f ca="1">IF(AA6&lt;0,0,INT(AA6/$AK$1))</f>
@@ -907,7 +907,7 @@
       </c>
       <c r="AB3" s="9">
         <f ca="1">IF(AB6&lt;0,0,INT(AB6/$AK$1))</f>
-        <v>3878</v>
+        <v>3857</v>
       </c>
       <c r="AE3" s="5">
         <f t="shared" ref="AE3:AE4" ca="1" si="12">SUM(C3,G3,K3,O3,S3,W3,AA3)</f>
@@ -915,7 +915,7 @@
       </c>
       <c r="AF3" s="5">
         <f ca="1">SUM(D3,H3,L3,P3,T3,X3,AB3)</f>
-        <v>32190</v>
+        <v>32750</v>
       </c>
       <c r="AI3" s="1">
         <v>41996</v>
@@ -925,7 +925,7 @@
       </c>
       <c r="AK3" s="2">
         <f ca="1">(AK2-AK1)/AK2</f>
-        <v>0.27272727272727271</v>
+        <v>0.30303030303030304</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -1003,19 +1003,19 @@
       </c>
       <c r="C5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-C6)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-D6)</f>
-        <v>-7821</v>
+        <v>-11328</v>
       </c>
       <c r="G5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-G6)</f>
-        <v>-19</v>
+        <v>-15</v>
       </c>
       <c r="H5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-H6)</f>
-        <v>-11083</v>
+        <v>-8687</v>
       </c>
       <c r="K5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-K6)</f>
@@ -1023,15 +1023,15 @@
       </c>
       <c r="L5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-L6)</f>
-        <v>4871</v>
+        <v>5222</v>
       </c>
       <c r="O5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-O6)</f>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="P5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-P6)</f>
-        <v>2542</v>
+        <v>-1388</v>
       </c>
       <c r="S5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-S6)</f>
@@ -1039,39 +1039,39 @@
       </c>
       <c r="T5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-T6)</f>
-        <v>-34529</v>
+        <v>-37246</v>
       </c>
       <c r="W5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-W6)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="X5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-X6)</f>
-        <v>1727</v>
+        <v>-2329</v>
       </c>
       <c r="AA5" s="9">
         <f ca="1">IF(150-INT(150-150/34*$AK$1)&lt;0,0,150-INT(150-150/34*$AK$1)-AA6)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="AB5" s="9">
         <f ca="1">IF(150000-INT(150000-150000/34*$AK$1)&lt;0,0,150000-INT(150000-150000/34*$AK$1)-AB6)</f>
-        <v>12805</v>
+        <v>12741</v>
       </c>
       <c r="AE5" s="5">
         <f ca="1">SUM(C5,G5,K5,O5,S5,W5,AA5)</f>
-        <v>-13</v>
+        <v>-16</v>
       </c>
       <c r="AF5" s="5">
         <f ca="1">SUM(D5,H5,L5,P5,T5,X5,AB5)</f>
-        <v>-31488</v>
+        <v>-43015</v>
       </c>
       <c r="AG5" s="3">
         <f ca="1">-$AK$3+AG6</f>
-        <v>8.2251082251082464E-3</v>
+        <v>1.7316017316017507E-3</v>
       </c>
       <c r="AH5" s="3">
         <f ca="1">AH6-$AK$3</f>
-        <v>-8.6025108225107894E-3</v>
+        <v>-2.0470303030303061E-2</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -1080,75 +1080,75 @@
       </c>
       <c r="C6" s="9">
         <f>IF(150-C11&lt;0,0,150-C11)</f>
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D6" s="9">
         <f>IF(150000-D11&lt;0,0,150000-D11)</f>
-        <v>113704</v>
+        <v>112799</v>
       </c>
       <c r="G6" s="9">
         <f>IF(150-G11&lt;0,0,150-G11)</f>
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="H6" s="9">
         <f>IF(150000-H11&lt;0,0,150000-H11)</f>
-        <v>116966</v>
+        <v>110158</v>
       </c>
       <c r="K6" s="9">
         <f>IF(150-K11&lt;0,0,150-K11)</f>
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="L6" s="9">
         <f>IF(150000-L11&lt;0,0,150000-L11)</f>
-        <v>101012</v>
+        <v>96249</v>
       </c>
       <c r="O6" s="9">
         <f>IF(150-O11&lt;0,0,150-O11)</f>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P6" s="9">
         <f>IF(150000-P11&lt;0,0,150000-P11)</f>
-        <v>103341</v>
+        <v>102859</v>
       </c>
       <c r="S6" s="9">
         <f>IF(150-S11&lt;0,0,150-S11)</f>
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="T6" s="9">
         <f>IF(150000-T11&lt;0,0,150000-T11)</f>
-        <v>140412</v>
+        <v>138717</v>
       </c>
       <c r="W6" s="9">
         <f>IF(150-W11&lt;0,0,150-W11)</f>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X6" s="9">
         <f>IF(150000-X11&lt;0,0,150000-X11)</f>
-        <v>104156</v>
+        <v>103800</v>
       </c>
       <c r="AA6" s="9">
         <f>IF(150-AA11&lt;0,0,150-AA11)</f>
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AB6" s="9">
         <f>IF(150000-AB11&lt;0,0,150000-AB11)</f>
-        <v>93078</v>
+        <v>88730</v>
       </c>
       <c r="AE6" s="5">
         <f>SUM(C6,G6,K6,O6,S6,W6,AA6)</f>
-        <v>755</v>
+        <v>730</v>
       </c>
       <c r="AF6" s="5">
         <f>SUM(D6,H6,L6,P6,T6,X6,AB6)</f>
-        <v>772669</v>
+        <v>753312</v>
       </c>
       <c r="AG6" s="3">
         <f>(7*150-AE6)/(7*150)</f>
-        <v>0.28095238095238095</v>
+        <v>0.30476190476190479</v>
       </c>
       <c r="AH6" s="3">
         <f>(7*150000-AF6)/(7*150000)</f>
-        <v>0.26412476190476192</v>
+        <v>0.28255999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:37">
@@ -1157,11 +1157,11 @@
       </c>
       <c r="AE7" s="5">
         <f>150*7-AE6</f>
-        <v>295</v>
+        <v>320</v>
       </c>
       <c r="AF7" s="5">
         <f>150000*7-AF6</f>
-        <v>277331</v>
+        <v>296688</v>
       </c>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
@@ -1282,11 +1282,11 @@
       </c>
       <c r="C11" s="13">
         <f t="shared" ref="C11:P26" si="14">C12</f>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D11" s="14">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E11" s="16">
         <f t="shared" ref="E11:E39" si="15">C11-C12</f>
@@ -1298,11 +1298,11 @@
       </c>
       <c r="G11" s="13">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H11" s="14">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I11" s="16">
         <f t="shared" ref="I11:I39" si="17">G11-G12</f>
@@ -1314,11 +1314,11 @@
       </c>
       <c r="K11" s="13">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L11" s="14">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M11" s="16">
         <f t="shared" ref="M11:M39" si="19">K11-K12</f>
@@ -1330,11 +1330,11 @@
       </c>
       <c r="O11" s="13">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P11" s="14">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q11" s="16">
         <f t="shared" ref="Q11:Q39" si="21">O11-O12</f>
@@ -1346,11 +1346,11 @@
       </c>
       <c r="S11" s="13">
         <f t="shared" ref="S11:AB32" si="23">S12</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T11" s="14">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U11" s="16">
         <f t="shared" ref="U11:U39" si="24">S11-S12</f>
@@ -1362,11 +1362,11 @@
       </c>
       <c r="W11" s="13">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X11" s="14">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y11" s="16">
         <f t="shared" ref="Y11:Y39" si="26">W11-W12</f>
@@ -1378,11 +1378,11 @@
       </c>
       <c r="AA11" s="13">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB11" s="14">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC11" s="16">
         <f t="shared" ref="AC11:AC39" si="28">AA11-AA12</f>
@@ -1410,11 +1410,11 @@
       </c>
       <c r="C12" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D12" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E12" s="16">
         <f t="shared" si="15"/>
@@ -1426,11 +1426,11 @@
       </c>
       <c r="G12" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H12" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I12" s="16">
         <f t="shared" si="17"/>
@@ -1442,11 +1442,11 @@
       </c>
       <c r="K12" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L12" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M12" s="16">
         <f t="shared" si="19"/>
@@ -1458,11 +1458,11 @@
       </c>
       <c r="O12" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P12" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q12" s="16">
         <f t="shared" si="21"/>
@@ -1474,11 +1474,11 @@
       </c>
       <c r="S12" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T12" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U12" s="16">
         <f t="shared" si="24"/>
@@ -1490,11 +1490,11 @@
       </c>
       <c r="W12" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X12" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y12" s="16">
         <f t="shared" si="26"/>
@@ -1506,11 +1506,11 @@
       </c>
       <c r="AA12" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB12" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC12" s="16">
         <f t="shared" si="28"/>
@@ -1538,11 +1538,11 @@
       </c>
       <c r="C13" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E13" s="16">
         <f t="shared" si="15"/>
@@ -1554,11 +1554,11 @@
       </c>
       <c r="G13" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H13" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I13" s="16">
         <f t="shared" si="17"/>
@@ -1570,11 +1570,11 @@
       </c>
       <c r="K13" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L13" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M13" s="16">
         <f t="shared" si="19"/>
@@ -1586,11 +1586,11 @@
       </c>
       <c r="O13" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P13" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q13" s="16">
         <f t="shared" si="21"/>
@@ -1602,11 +1602,11 @@
       </c>
       <c r="S13" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T13" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U13" s="16">
         <f t="shared" si="24"/>
@@ -1618,11 +1618,11 @@
       </c>
       <c r="W13" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X13" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y13" s="16">
         <f t="shared" si="26"/>
@@ -1634,11 +1634,11 @@
       </c>
       <c r="AA13" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB13" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC13" s="16">
         <f t="shared" si="28"/>
@@ -1666,11 +1666,11 @@
       </c>
       <c r="C14" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" si="15"/>
@@ -1682,11 +1682,11 @@
       </c>
       <c r="G14" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H14" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I14" s="16">
         <f t="shared" si="17"/>
@@ -1698,11 +1698,11 @@
       </c>
       <c r="K14" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L14" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M14" s="16">
         <f t="shared" si="19"/>
@@ -1714,11 +1714,11 @@
       </c>
       <c r="O14" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P14" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q14" s="16">
         <f t="shared" si="21"/>
@@ -1730,11 +1730,11 @@
       </c>
       <c r="S14" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T14" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U14" s="16">
         <f t="shared" si="24"/>
@@ -1746,11 +1746,11 @@
       </c>
       <c r="W14" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X14" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y14" s="16">
         <f t="shared" si="26"/>
@@ -1762,11 +1762,11 @@
       </c>
       <c r="AA14" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB14" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC14" s="16">
         <f t="shared" si="28"/>
@@ -1794,11 +1794,11 @@
       </c>
       <c r="C15" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E15" s="16">
         <f t="shared" si="15"/>
@@ -1810,11 +1810,11 @@
       </c>
       <c r="G15" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H15" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I15" s="16">
         <f t="shared" si="17"/>
@@ -1826,11 +1826,11 @@
       </c>
       <c r="K15" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L15" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M15" s="16">
         <f t="shared" si="19"/>
@@ -1842,11 +1842,11 @@
       </c>
       <c r="O15" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P15" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q15" s="16">
         <f t="shared" si="21"/>
@@ -1858,11 +1858,11 @@
       </c>
       <c r="S15" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T15" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U15" s="16">
         <f t="shared" si="24"/>
@@ -1874,11 +1874,11 @@
       </c>
       <c r="W15" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X15" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y15" s="16">
         <f t="shared" si="26"/>
@@ -1890,11 +1890,11 @@
       </c>
       <c r="AA15" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB15" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC15" s="16">
         <f t="shared" si="28"/>
@@ -1922,11 +1922,11 @@
       </c>
       <c r="C16" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E16" s="16">
         <f t="shared" si="15"/>
@@ -1938,11 +1938,11 @@
       </c>
       <c r="G16" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H16" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I16" s="16">
         <f t="shared" si="17"/>
@@ -1954,11 +1954,11 @@
       </c>
       <c r="K16" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L16" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M16" s="16">
         <f t="shared" si="19"/>
@@ -1970,11 +1970,11 @@
       </c>
       <c r="O16" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P16" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q16" s="16">
         <f t="shared" si="21"/>
@@ -1986,11 +1986,11 @@
       </c>
       <c r="S16" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T16" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U16" s="16">
         <f t="shared" si="24"/>
@@ -2002,11 +2002,11 @@
       </c>
       <c r="W16" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X16" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y16" s="16">
         <f t="shared" si="26"/>
@@ -2018,11 +2018,11 @@
       </c>
       <c r="AA16" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB16" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC16" s="16">
         <f t="shared" si="28"/>
@@ -2050,11 +2050,11 @@
       </c>
       <c r="C17" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E17" s="16">
         <f t="shared" si="15"/>
@@ -2066,11 +2066,11 @@
       </c>
       <c r="G17" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H17" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I17" s="16">
         <f t="shared" si="17"/>
@@ -2082,11 +2082,11 @@
       </c>
       <c r="K17" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L17" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M17" s="16">
         <f t="shared" si="19"/>
@@ -2098,11 +2098,11 @@
       </c>
       <c r="O17" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P17" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q17" s="16">
         <f t="shared" si="21"/>
@@ -2114,11 +2114,11 @@
       </c>
       <c r="S17" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T17" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U17" s="16">
         <f t="shared" si="24"/>
@@ -2130,11 +2130,11 @@
       </c>
       <c r="W17" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X17" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y17" s="16">
         <f t="shared" si="26"/>
@@ -2146,11 +2146,11 @@
       </c>
       <c r="AA17" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB17" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC17" s="16">
         <f t="shared" si="28"/>
@@ -2178,11 +2178,11 @@
       </c>
       <c r="C18" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E18" s="16">
         <f t="shared" si="15"/>
@@ -2194,11 +2194,11 @@
       </c>
       <c r="G18" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H18" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I18" s="16">
         <f t="shared" si="17"/>
@@ -2210,11 +2210,11 @@
       </c>
       <c r="K18" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L18" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M18" s="16">
         <f t="shared" si="19"/>
@@ -2226,11 +2226,11 @@
       </c>
       <c r="O18" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P18" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q18" s="16">
         <f t="shared" si="21"/>
@@ -2242,11 +2242,11 @@
       </c>
       <c r="S18" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T18" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U18" s="16">
         <f t="shared" si="24"/>
@@ -2258,11 +2258,11 @@
       </c>
       <c r="W18" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X18" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y18" s="16">
         <f t="shared" si="26"/>
@@ -2274,11 +2274,11 @@
       </c>
       <c r="AA18" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB18" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC18" s="16">
         <f t="shared" si="28"/>
@@ -2306,11 +2306,11 @@
       </c>
       <c r="C19" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E19" s="16">
         <f t="shared" si="15"/>
@@ -2322,11 +2322,11 @@
       </c>
       <c r="G19" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H19" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I19" s="16">
         <f t="shared" si="17"/>
@@ -2338,11 +2338,11 @@
       </c>
       <c r="K19" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L19" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M19" s="16">
         <f t="shared" si="19"/>
@@ -2354,11 +2354,11 @@
       </c>
       <c r="O19" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P19" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q19" s="16">
         <f t="shared" si="21"/>
@@ -2370,11 +2370,11 @@
       </c>
       <c r="S19" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T19" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U19" s="16">
         <f t="shared" si="24"/>
@@ -2386,11 +2386,11 @@
       </c>
       <c r="W19" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X19" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y19" s="16">
         <f t="shared" si="26"/>
@@ -2402,11 +2402,11 @@
       </c>
       <c r="AA19" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB19" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC19" s="16">
         <f t="shared" si="28"/>
@@ -2434,11 +2434,11 @@
       </c>
       <c r="C20" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D20" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E20" s="16">
         <f t="shared" si="15"/>
@@ -2450,11 +2450,11 @@
       </c>
       <c r="G20" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H20" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I20" s="16">
         <f t="shared" si="17"/>
@@ -2466,11 +2466,11 @@
       </c>
       <c r="K20" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L20" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M20" s="16">
         <f t="shared" si="19"/>
@@ -2482,11 +2482,11 @@
       </c>
       <c r="O20" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P20" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q20" s="16">
         <f t="shared" si="21"/>
@@ -2498,11 +2498,11 @@
       </c>
       <c r="S20" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T20" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U20" s="16">
         <f t="shared" si="24"/>
@@ -2514,11 +2514,11 @@
       </c>
       <c r="W20" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X20" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y20" s="16">
         <f t="shared" si="26"/>
@@ -2530,11 +2530,11 @@
       </c>
       <c r="AA20" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB20" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC20" s="16">
         <f t="shared" si="28"/>
@@ -2562,11 +2562,11 @@
       </c>
       <c r="C21" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E21" s="16">
         <f t="shared" si="15"/>
@@ -2578,11 +2578,11 @@
       </c>
       <c r="G21" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H21" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I21" s="16">
         <f t="shared" si="17"/>
@@ -2594,11 +2594,11 @@
       </c>
       <c r="K21" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L21" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M21" s="16">
         <f t="shared" si="19"/>
@@ -2610,11 +2610,11 @@
       </c>
       <c r="O21" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P21" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q21" s="16">
         <f t="shared" si="21"/>
@@ -2626,11 +2626,11 @@
       </c>
       <c r="S21" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T21" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U21" s="16">
         <f t="shared" si="24"/>
@@ -2642,11 +2642,11 @@
       </c>
       <c r="W21" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X21" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y21" s="16">
         <f t="shared" si="26"/>
@@ -2658,11 +2658,11 @@
       </c>
       <c r="AA21" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB21" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC21" s="16">
         <f t="shared" si="28"/>
@@ -2690,11 +2690,11 @@
       </c>
       <c r="C22" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D22" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E22" s="16">
         <f t="shared" si="15"/>
@@ -2706,11 +2706,11 @@
       </c>
       <c r="G22" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H22" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I22" s="16">
         <f t="shared" si="17"/>
@@ -2722,11 +2722,11 @@
       </c>
       <c r="K22" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L22" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M22" s="16">
         <f t="shared" si="19"/>
@@ -2738,11 +2738,11 @@
       </c>
       <c r="O22" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P22" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q22" s="16">
         <f t="shared" si="21"/>
@@ -2754,11 +2754,11 @@
       </c>
       <c r="S22" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T22" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U22" s="16">
         <f t="shared" si="24"/>
@@ -2770,11 +2770,11 @@
       </c>
       <c r="W22" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X22" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y22" s="16">
         <f t="shared" si="26"/>
@@ -2786,11 +2786,11 @@
       </c>
       <c r="AA22" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB22" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC22" s="16">
         <f t="shared" si="28"/>
@@ -2818,11 +2818,11 @@
       </c>
       <c r="C23" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E23" s="16">
         <f t="shared" si="15"/>
@@ -2834,11 +2834,11 @@
       </c>
       <c r="G23" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H23" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I23" s="16">
         <f t="shared" si="17"/>
@@ -2850,11 +2850,11 @@
       </c>
       <c r="K23" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L23" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M23" s="16">
         <f t="shared" si="19"/>
@@ -2866,11 +2866,11 @@
       </c>
       <c r="O23" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P23" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q23" s="16">
         <f t="shared" si="21"/>
@@ -2882,11 +2882,11 @@
       </c>
       <c r="S23" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T23" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U23" s="16">
         <f t="shared" si="24"/>
@@ -2898,11 +2898,11 @@
       </c>
       <c r="W23" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X23" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y23" s="16">
         <f t="shared" si="26"/>
@@ -2914,11 +2914,11 @@
       </c>
       <c r="AA23" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB23" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC23" s="16">
         <f t="shared" si="28"/>
@@ -2946,11 +2946,11 @@
       </c>
       <c r="C24" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D24" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E24" s="16">
         <f t="shared" si="15"/>
@@ -2962,11 +2962,11 @@
       </c>
       <c r="G24" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H24" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I24" s="16">
         <f t="shared" si="17"/>
@@ -2978,11 +2978,11 @@
       </c>
       <c r="K24" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L24" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M24" s="16">
         <f t="shared" si="19"/>
@@ -2994,11 +2994,11 @@
       </c>
       <c r="O24" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P24" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q24" s="16">
         <f t="shared" si="21"/>
@@ -3010,11 +3010,11 @@
       </c>
       <c r="S24" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T24" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U24" s="16">
         <f t="shared" si="24"/>
@@ -3026,11 +3026,11 @@
       </c>
       <c r="W24" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X24" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y24" s="16">
         <f t="shared" si="26"/>
@@ -3042,11 +3042,11 @@
       </c>
       <c r="AA24" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB24" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC24" s="16">
         <f t="shared" si="28"/>
@@ -3074,11 +3074,11 @@
       </c>
       <c r="C25" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D25" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E25" s="16">
         <f t="shared" si="15"/>
@@ -3090,11 +3090,11 @@
       </c>
       <c r="G25" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H25" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I25" s="16">
         <f t="shared" si="17"/>
@@ -3106,11 +3106,11 @@
       </c>
       <c r="K25" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L25" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M25" s="16">
         <f t="shared" si="19"/>
@@ -3122,11 +3122,11 @@
       </c>
       <c r="O25" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P25" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q25" s="16">
         <f t="shared" si="21"/>
@@ -3138,11 +3138,11 @@
       </c>
       <c r="S25" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T25" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U25" s="16">
         <f t="shared" si="24"/>
@@ -3154,11 +3154,11 @@
       </c>
       <c r="W25" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X25" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y25" s="16">
         <f t="shared" si="26"/>
@@ -3170,11 +3170,11 @@
       </c>
       <c r="AA25" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB25" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC25" s="16">
         <f t="shared" si="28"/>
@@ -3202,11 +3202,11 @@
       </c>
       <c r="C26" s="15">
         <f t="shared" si="14"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D26" s="16">
         <f t="shared" si="14"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E26" s="16">
         <f t="shared" si="15"/>
@@ -3218,11 +3218,11 @@
       </c>
       <c r="G26" s="15">
         <f t="shared" si="14"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H26" s="16">
         <f t="shared" si="14"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I26" s="16">
         <f t="shared" si="17"/>
@@ -3234,11 +3234,11 @@
       </c>
       <c r="K26" s="15">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L26" s="16">
         <f t="shared" si="14"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M26" s="16">
         <f t="shared" si="19"/>
@@ -3250,11 +3250,11 @@
       </c>
       <c r="O26" s="15">
         <f t="shared" si="14"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P26" s="16">
         <f t="shared" si="14"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q26" s="16">
         <f t="shared" si="21"/>
@@ -3266,11 +3266,11 @@
       </c>
       <c r="S26" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T26" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U26" s="16">
         <f t="shared" si="24"/>
@@ -3282,11 +3282,11 @@
       </c>
       <c r="W26" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X26" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y26" s="16">
         <f t="shared" si="26"/>
@@ -3298,11 +3298,11 @@
       </c>
       <c r="AA26" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB26" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC26" s="16">
         <f t="shared" si="28"/>
@@ -3330,11 +3330,11 @@
       </c>
       <c r="C27" s="15">
         <f t="shared" ref="C27:P40" si="31">C28</f>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E27" s="16">
         <f t="shared" si="15"/>
@@ -3346,11 +3346,11 @@
       </c>
       <c r="G27" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H27" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I27" s="16">
         <f t="shared" si="17"/>
@@ -3362,11 +3362,11 @@
       </c>
       <c r="K27" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L27" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M27" s="16">
         <f t="shared" si="19"/>
@@ -3378,11 +3378,11 @@
       </c>
       <c r="O27" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P27" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q27" s="16">
         <f t="shared" si="21"/>
@@ -3394,11 +3394,11 @@
       </c>
       <c r="S27" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T27" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U27" s="16">
         <f t="shared" si="24"/>
@@ -3410,11 +3410,11 @@
       </c>
       <c r="W27" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X27" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y27" s="16">
         <f t="shared" si="26"/>
@@ -3426,11 +3426,11 @@
       </c>
       <c r="AA27" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB27" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC27" s="16">
         <f t="shared" si="28"/>
@@ -3458,11 +3458,11 @@
       </c>
       <c r="C28" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D28" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E28" s="16">
         <f t="shared" si="15"/>
@@ -3474,11 +3474,11 @@
       </c>
       <c r="G28" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H28" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I28" s="16">
         <f t="shared" si="17"/>
@@ -3490,11 +3490,11 @@
       </c>
       <c r="K28" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L28" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M28" s="16">
         <f t="shared" si="19"/>
@@ -3506,11 +3506,11 @@
       </c>
       <c r="O28" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P28" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q28" s="16">
         <f t="shared" si="21"/>
@@ -3522,11 +3522,11 @@
       </c>
       <c r="S28" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T28" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U28" s="16">
         <f t="shared" si="24"/>
@@ -3538,11 +3538,11 @@
       </c>
       <c r="W28" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X28" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y28" s="16">
         <f t="shared" si="26"/>
@@ -3554,11 +3554,11 @@
       </c>
       <c r="AA28" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB28" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC28" s="16">
         <f t="shared" si="28"/>
@@ -3586,11 +3586,11 @@
       </c>
       <c r="C29" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D29" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E29" s="16">
         <f t="shared" si="15"/>
@@ -3602,11 +3602,11 @@
       </c>
       <c r="G29" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H29" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I29" s="16">
         <f t="shared" si="17"/>
@@ -3618,11 +3618,11 @@
       </c>
       <c r="K29" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L29" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M29" s="16">
         <f t="shared" si="19"/>
@@ -3634,11 +3634,11 @@
       </c>
       <c r="O29" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P29" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q29" s="16">
         <f t="shared" si="21"/>
@@ -3650,11 +3650,11 @@
       </c>
       <c r="S29" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T29" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U29" s="16">
         <f t="shared" si="24"/>
@@ -3666,11 +3666,11 @@
       </c>
       <c r="W29" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X29" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y29" s="16">
         <f t="shared" si="26"/>
@@ -3682,11 +3682,11 @@
       </c>
       <c r="AA29" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB29" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC29" s="16">
         <f t="shared" si="28"/>
@@ -3714,11 +3714,11 @@
       </c>
       <c r="C30" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D30" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E30" s="16">
         <f t="shared" si="15"/>
@@ -3730,11 +3730,11 @@
       </c>
       <c r="G30" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H30" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I30" s="16">
         <f t="shared" si="17"/>
@@ -3746,11 +3746,11 @@
       </c>
       <c r="K30" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L30" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M30" s="16">
         <f t="shared" si="19"/>
@@ -3762,11 +3762,11 @@
       </c>
       <c r="O30" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P30" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q30" s="16">
         <f t="shared" si="21"/>
@@ -3778,11 +3778,11 @@
       </c>
       <c r="S30" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T30" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U30" s="16">
         <f t="shared" si="24"/>
@@ -3794,11 +3794,11 @@
       </c>
       <c r="W30" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X30" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y30" s="16">
         <f t="shared" si="26"/>
@@ -3810,11 +3810,11 @@
       </c>
       <c r="AA30" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB30" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC30" s="16">
         <f t="shared" si="28"/>
@@ -3842,11 +3842,11 @@
       </c>
       <c r="C31" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E31" s="16">
         <f t="shared" si="15"/>
@@ -3858,11 +3858,11 @@
       </c>
       <c r="G31" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H31" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I31" s="16">
         <f t="shared" si="17"/>
@@ -3874,11 +3874,11 @@
       </c>
       <c r="K31" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L31" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M31" s="16">
         <f t="shared" si="19"/>
@@ -3890,11 +3890,11 @@
       </c>
       <c r="O31" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P31" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q31" s="16">
         <f t="shared" si="21"/>
@@ -3906,11 +3906,11 @@
       </c>
       <c r="S31" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T31" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U31" s="16">
         <f t="shared" si="24"/>
@@ -3922,11 +3922,11 @@
       </c>
       <c r="W31" s="15">
         <f t="shared" si="23"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X31" s="16">
         <f t="shared" si="23"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y31" s="16">
         <f t="shared" si="26"/>
@@ -3938,11 +3938,11 @@
       </c>
       <c r="AA31" s="15">
         <f t="shared" si="23"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB31" s="16">
         <f t="shared" si="23"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC31" s="16">
         <f t="shared" si="28"/>
@@ -3970,11 +3970,11 @@
       </c>
       <c r="C32" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D32" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E32" s="16">
         <f t="shared" si="15"/>
@@ -3986,11 +3986,11 @@
       </c>
       <c r="G32" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H32" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I32" s="16">
         <f t="shared" si="17"/>
@@ -4002,11 +4002,11 @@
       </c>
       <c r="K32" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L32" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M32" s="16">
         <f t="shared" si="19"/>
@@ -4018,11 +4018,11 @@
       </c>
       <c r="O32" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P32" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q32" s="16">
         <f t="shared" si="21"/>
@@ -4034,11 +4034,11 @@
       </c>
       <c r="S32" s="15">
         <f t="shared" si="23"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T32" s="16">
         <f t="shared" si="23"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U32" s="16">
         <f t="shared" si="24"/>
@@ -4050,11 +4050,11 @@
       </c>
       <c r="W32" s="15">
         <f t="shared" ref="W32:AB37" si="33">W33</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X32" s="16">
         <f t="shared" si="33"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y32" s="16">
         <f t="shared" si="26"/>
@@ -4066,11 +4066,11 @@
       </c>
       <c r="AA32" s="15">
         <f t="shared" si="33"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB32" s="16">
         <f t="shared" si="33"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC32" s="16">
         <f t="shared" si="28"/>
@@ -4098,11 +4098,11 @@
       </c>
       <c r="C33" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D33" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E33" s="16">
         <f t="shared" si="15"/>
@@ -4114,11 +4114,11 @@
       </c>
       <c r="G33" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H33" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I33" s="16">
         <f t="shared" si="17"/>
@@ -4130,11 +4130,11 @@
       </c>
       <c r="K33" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L33" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M33" s="16">
         <f t="shared" si="19"/>
@@ -4146,11 +4146,11 @@
       </c>
       <c r="O33" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P33" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q33" s="16">
         <f t="shared" si="21"/>
@@ -4162,11 +4162,11 @@
       </c>
       <c r="S33" s="15">
         <f t="shared" ref="S33:T39" si="34">S34</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T33" s="16">
         <f t="shared" si="34"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U33" s="16">
         <f t="shared" si="24"/>
@@ -4178,11 +4178,11 @@
       </c>
       <c r="W33" s="15">
         <f t="shared" si="33"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X33" s="16">
         <f t="shared" si="33"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y33" s="16">
         <f t="shared" si="26"/>
@@ -4194,11 +4194,11 @@
       </c>
       <c r="AA33" s="15">
         <f t="shared" si="33"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB33" s="16">
         <f t="shared" si="33"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC33" s="16">
         <f t="shared" si="28"/>
@@ -4226,11 +4226,11 @@
       </c>
       <c r="C34" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D34" s="16">
         <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E34" s="16">
         <f t="shared" si="15"/>
@@ -4242,11 +4242,11 @@
       </c>
       <c r="G34" s="15">
         <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H34" s="16">
         <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I34" s="16">
         <f t="shared" si="17"/>
@@ -4258,11 +4258,11 @@
       </c>
       <c r="K34" s="15">
         <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L34" s="16">
         <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M34" s="16">
         <f t="shared" si="19"/>
@@ -4274,11 +4274,11 @@
       </c>
       <c r="O34" s="15">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P34" s="16">
         <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q34" s="16">
         <f t="shared" si="21"/>
@@ -4290,11 +4290,11 @@
       </c>
       <c r="S34" s="15">
         <f t="shared" si="34"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T34" s="16">
         <f t="shared" si="34"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U34" s="16">
         <f t="shared" si="24"/>
@@ -4306,11 +4306,11 @@
       </c>
       <c r="W34" s="15">
         <f t="shared" si="33"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X34" s="16">
         <f t="shared" si="33"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y34" s="16">
         <f t="shared" si="26"/>
@@ -4322,11 +4322,11 @@
       </c>
       <c r="AA34" s="15">
         <f t="shared" si="33"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB34" s="16">
         <f t="shared" si="33"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC34" s="16">
         <f t="shared" si="28"/>
@@ -4345,7 +4345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:36" hidden="1">
+    <row r="35" spans="1:36">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -4354,11 +4354,10 @@
       </c>
       <c r="C35" s="15">
         <f t="shared" si="31"/>
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D35" s="16">
-        <f t="shared" si="31"/>
-        <v>36296</v>
+        <v>37201</v>
       </c>
       <c r="E35" s="16">
         <f t="shared" si="15"/>
@@ -4366,111 +4365,99 @@
       </c>
       <c r="F35" s="17">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="15">
-        <f t="shared" si="31"/>
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H35" s="16">
-        <f t="shared" si="31"/>
-        <v>33034</v>
+        <v>39842</v>
       </c>
       <c r="I35" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J35" s="17">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2155</v>
       </c>
       <c r="K35" s="15">
-        <f t="shared" si="31"/>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="L35" s="16">
-        <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>53751</v>
       </c>
       <c r="M35" s="16">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N35" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1981</v>
       </c>
       <c r="O35" s="15">
-        <f t="shared" si="31"/>
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="P35" s="16">
-        <f t="shared" si="31"/>
-        <v>46659</v>
+        <v>47141</v>
       </c>
       <c r="Q35" s="16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35" s="17">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>482</v>
       </c>
       <c r="S35" s="15">
-        <f t="shared" si="34"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="T35" s="16">
-        <f t="shared" si="34"/>
-        <v>9588</v>
+        <v>11283</v>
       </c>
       <c r="U35" s="16">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V35" s="17">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1695</v>
       </c>
       <c r="W35" s="15">
-        <f t="shared" si="33"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X35" s="16">
-        <f t="shared" si="33"/>
-        <v>45844</v>
+        <v>46200</v>
       </c>
       <c r="Y35" s="16">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z35" s="17">
         <f t="shared" si="27"/>
-        <v>0</v>
+        <v>356</v>
       </c>
       <c r="AA35" s="15">
-        <f t="shared" si="33"/>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB35" s="16">
-        <f t="shared" si="33"/>
-        <v>56922</v>
+        <v>61270</v>
       </c>
       <c r="AC35" s="16">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD35" s="17">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>4348</v>
       </c>
       <c r="AE35" s="4">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AF35" s="4">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>11018</v>
       </c>
     </row>
     <row r="36" spans="1:36">
@@ -4481,48 +4468,46 @@
         <v>41998</v>
       </c>
       <c r="C36" s="15">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="D36" s="16">
-        <v>36296</v>
+        <v>37200</v>
       </c>
       <c r="E36" s="16">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F36" s="17">
         <f t="shared" si="16"/>
-        <v>2396</v>
+        <v>3300</v>
       </c>
       <c r="G36" s="15">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H36" s="16">
-        <v>33034</v>
+        <v>37687</v>
       </c>
       <c r="I36" s="16">
         <f t="shared" si="17"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J36" s="17">
         <f t="shared" si="18"/>
-        <v>18635</v>
+        <v>23288</v>
       </c>
       <c r="K36" s="15">
-        <f t="shared" si="31"/>
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="L36" s="16">
-        <f t="shared" si="31"/>
-        <v>48988</v>
+        <v>51770</v>
       </c>
       <c r="M36" s="16">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N36" s="17">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="O36" s="15">
         <v>68</v>
@@ -4582,11 +4567,26 @@
       </c>
       <c r="AE36" s="4">
         <f t="shared" si="32"/>
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="AF36" s="4">
         <f t="shared" si="32"/>
-        <v>32329</v>
+        <v>40668</v>
+      </c>
+      <c r="AG36">
+        <v>16592</v>
+      </c>
+      <c r="AH36">
+        <f t="shared" ref="AH36" si="35">AG36-AG37</f>
+        <v>56</v>
+      </c>
+      <c r="AI36">
+        <f t="shared" ref="AI36" si="36">AE36/$AH36</f>
+        <v>0.9642857142857143</v>
+      </c>
+      <c r="AJ36">
+        <f t="shared" ref="AJ36" si="37">AF36/$AH36</f>
+        <v>726.21428571428567</v>
       </c>
     </row>
     <row r="37" spans="1:36">
@@ -4711,15 +4711,15 @@
         <v>16536</v>
       </c>
       <c r="AH37">
-        <f t="shared" ref="AH37:AH38" si="35">AG37-AG38</f>
+        <f t="shared" ref="AH37:AH38" si="38">AG37-AG38</f>
         <v>22</v>
       </c>
       <c r="AI37">
-        <f t="shared" ref="AI37:AJ40" si="36">AE37/$AH37</f>
+        <f t="shared" ref="AI37:AJ40" si="39">AE37/$AH37</f>
         <v>1.1363636363636365</v>
       </c>
       <c r="AJ37">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1342.409090909091</v>
       </c>
     </row>
@@ -4844,15 +4844,15 @@
         <v>16514</v>
       </c>
       <c r="AH38">
-        <f t="shared" si="35"/>
+        <f t="shared" si="38"/>
         <v>27</v>
       </c>
       <c r="AI38">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>0.77777777777777779</v>
       </c>
       <c r="AJ38">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>494.74074074074076</v>
       </c>
     </row>
@@ -4983,11 +4983,11 @@
         <v>10</v>
       </c>
       <c r="AI39">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.4</v>
       </c>
       <c r="AJ39">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>793</v>
       </c>
     </row>
@@ -5113,11 +5113,11 @@
         <v>28</v>
       </c>
       <c r="AI40">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1.7142857142857142</v>
       </c>
       <c r="AJ40">
-        <f t="shared" si="36"/>
+        <f t="shared" si="39"/>
         <v>1449.1071428571429</v>
       </c>
     </row>
@@ -5252,26 +5252,26 @@
         <v>17472</v>
       </c>
       <c r="E42" s="16">
-        <f t="shared" ref="E42:F44" si="37">C42-C43</f>
+        <f t="shared" ref="E42:F44" si="40">C42-C43</f>
         <v>4</v>
       </c>
       <c r="F42" s="17">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>3603</v>
       </c>
       <c r="G42" s="15">
-        <f t="shared" ref="G42:T43" si="38">G43</f>
+        <f t="shared" ref="G42:T43" si="41">G43</f>
         <v>0</v>
       </c>
       <c r="H42" s="16">
         <v>2587</v>
       </c>
       <c r="I42" s="16">
-        <f t="shared" ref="I42:J44" si="39">G42-G43</f>
+        <f t="shared" ref="I42:J44" si="42">G42-G43</f>
         <v>0</v>
       </c>
       <c r="J42" s="17">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>2121</v>
       </c>
       <c r="K42" s="15">
@@ -5281,11 +5281,11 @@
         <v>17845</v>
       </c>
       <c r="M42" s="16">
-        <f t="shared" ref="M42:N44" si="40">K42-K43</f>
+        <f t="shared" ref="M42:N44" si="43">K42-K43</f>
         <v>0</v>
       </c>
       <c r="N42" s="17">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>1145</v>
       </c>
       <c r="O42" s="15">
@@ -5295,26 +5295,26 @@
         <v>15917</v>
       </c>
       <c r="Q42" s="16">
-        <f t="shared" ref="Q42:R44" si="41">O42-O43</f>
+        <f t="shared" ref="Q42:R44" si="44">O42-O43</f>
         <v>2</v>
       </c>
       <c r="R42" s="17">
+        <f t="shared" si="44"/>
+        <v>2510</v>
+      </c>
+      <c r="S42" s="15">
         <f t="shared" si="41"/>
-        <v>2510</v>
-      </c>
-      <c r="S42" s="15">
-        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="T42" s="16">
         <v>0</v>
       </c>
       <c r="U42" s="16">
-        <f t="shared" ref="U42:V44" si="42">S42-S43</f>
+        <f t="shared" ref="U42:V44" si="45">S42-S43</f>
         <v>0</v>
       </c>
       <c r="V42" s="17">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="W42" s="15">
@@ -5324,11 +5324,11 @@
         <v>6800</v>
       </c>
       <c r="Y42" s="16">
-        <f t="shared" ref="Y42:Z44" si="43">W42-W43</f>
+        <f t="shared" ref="Y42:Z44" si="46">W42-W43</f>
         <v>5</v>
       </c>
       <c r="Z42" s="17">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>2138</v>
       </c>
       <c r="AA42" s="15">
@@ -5338,11 +5338,11 @@
         <v>19779</v>
       </c>
       <c r="AC42" s="16">
-        <f t="shared" ref="AC42:AD44" si="44">AA42-AA43</f>
+        <f t="shared" ref="AC42:AD44" si="47">AA42-AA43</f>
         <v>6</v>
       </c>
       <c r="AD42" s="17">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>8542</v>
       </c>
       <c r="AE42" s="4">
@@ -5368,26 +5368,26 @@
         <v>13869</v>
       </c>
       <c r="E43" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>10</v>
       </c>
       <c r="F43" s="17">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>5719</v>
       </c>
       <c r="G43" s="15">
-        <f t="shared" si="38"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="H43" s="16">
         <v>466</v>
       </c>
       <c r="I43" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J43" s="17">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>466</v>
       </c>
       <c r="K43" s="15">
@@ -5397,11 +5397,11 @@
         <v>16700</v>
       </c>
       <c r="M43" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>2</v>
       </c>
       <c r="N43" s="17">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>14</v>
       </c>
       <c r="O43" s="15">
@@ -5411,27 +5411,27 @@
         <v>13407</v>
       </c>
       <c r="Q43" s="16">
+        <f t="shared" si="44"/>
+        <v>12</v>
+      </c>
+      <c r="R43" s="17">
+        <f t="shared" si="44"/>
+        <v>7199</v>
+      </c>
+      <c r="S43" s="15">
         <f t="shared" si="41"/>
-        <v>12</v>
-      </c>
-      <c r="R43" s="17">
+        <v>0</v>
+      </c>
+      <c r="T43" s="16">
         <f t="shared" si="41"/>
-        <v>7199</v>
-      </c>
-      <c r="S43" s="15">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="T43" s="16">
-        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="U43" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V43" s="17">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="W43" s="15">
@@ -5441,11 +5441,11 @@
         <v>4662</v>
       </c>
       <c r="Y43" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>3</v>
       </c>
       <c r="Z43" s="17">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>3582</v>
       </c>
       <c r="AA43" s="15">
@@ -5455,11 +5455,11 @@
         <v>11237</v>
       </c>
       <c r="AC43" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="AD43" s="17">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>1879</v>
       </c>
       <c r="AE43" s="4">
@@ -5485,11 +5485,11 @@
         <v>8150</v>
       </c>
       <c r="E44" s="16">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="F44" s="17">
-        <f t="shared" si="37"/>
+        <f t="shared" si="40"/>
         <v>4075</v>
       </c>
       <c r="G44" s="15">
@@ -5499,11 +5499,11 @@
         <v>0</v>
       </c>
       <c r="I44" s="16">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="J44" s="17">
-        <f t="shared" si="39"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="K44" s="15">
@@ -5513,11 +5513,11 @@
         <v>16686</v>
       </c>
       <c r="M44" s="16">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>8</v>
       </c>
       <c r="N44" s="17">
-        <f t="shared" si="40"/>
+        <f t="shared" si="43"/>
         <v>8343</v>
       </c>
       <c r="O44" s="15">
@@ -5527,11 +5527,11 @@
         <v>6208</v>
       </c>
       <c r="Q44" s="16">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>5</v>
       </c>
       <c r="R44" s="17">
-        <f t="shared" si="41"/>
+        <f t="shared" si="44"/>
         <v>3104</v>
       </c>
       <c r="S44" s="15">
@@ -5541,11 +5541,11 @@
         <v>0</v>
       </c>
       <c r="U44" s="16">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V44" s="17">
-        <f t="shared" si="42"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="W44" s="15">
@@ -5555,11 +5555,11 @@
         <v>1080</v>
       </c>
       <c r="Y44" s="16">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="Z44" s="17">
-        <f t="shared" si="43"/>
+        <f t="shared" si="46"/>
         <v>540</v>
       </c>
       <c r="AA44" s="15">
@@ -5569,11 +5569,11 @@
         <v>9358</v>
       </c>
       <c r="AC44" s="16">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>2</v>
       </c>
       <c r="AD44" s="17">
-        <f t="shared" si="44"/>
+        <f t="shared" si="47"/>
         <v>4679</v>
       </c>
       <c r="AE44" s="4">
@@ -5609,11 +5609,11 @@
         <v>4075</v>
       </c>
       <c r="G45" s="15">
-        <f t="shared" ref="G45:H45" si="45">INT(G44/2)</f>
+        <f t="shared" ref="G45:H45" si="48">INT(G44/2)</f>
         <v>0</v>
       </c>
       <c r="H45" s="16">
-        <f t="shared" si="45"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="I45" s="16">
@@ -5625,11 +5625,11 @@
         <v>0</v>
       </c>
       <c r="K45" s="15">
-        <f t="shared" ref="K45:L45" si="46">INT(K44/2)</f>
+        <f t="shared" ref="K45:L45" si="49">INT(K44/2)</f>
         <v>7</v>
       </c>
       <c r="L45" s="16">
-        <f t="shared" si="46"/>
+        <f t="shared" si="49"/>
         <v>8343</v>
       </c>
       <c r="M45" s="16">
@@ -5641,11 +5641,11 @@
         <v>8343</v>
       </c>
       <c r="O45" s="15">
-        <f t="shared" ref="O45:P45" si="47">INT(O44/2)</f>
+        <f t="shared" ref="O45:P45" si="50">INT(O44/2)</f>
         <v>4</v>
       </c>
       <c r="P45" s="16">
-        <f t="shared" si="47"/>
+        <f t="shared" si="50"/>
         <v>3104</v>
       </c>
       <c r="Q45" s="16">
@@ -5657,11 +5657,11 @@
         <v>3104</v>
       </c>
       <c r="S45" s="15">
-        <f t="shared" ref="S45:T45" si="48">INT(S44/2)</f>
+        <f t="shared" ref="S45:T45" si="51">INT(S44/2)</f>
         <v>0</v>
       </c>
       <c r="T45" s="16">
-        <f t="shared" si="48"/>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="U45" s="16">
@@ -5673,11 +5673,11 @@
         <v>0</v>
       </c>
       <c r="W45" s="15">
-        <f t="shared" ref="W45:X45" si="49">INT(W44/2)</f>
+        <f t="shared" ref="W45:X45" si="52">INT(W44/2)</f>
         <v>1</v>
       </c>
       <c r="X45" s="16">
-        <f t="shared" si="49"/>
+        <f t="shared" si="52"/>
         <v>540</v>
       </c>
       <c r="Y45" s="16">
@@ -5689,11 +5689,11 @@
         <v>540</v>
       </c>
       <c r="AA45" s="15">
-        <f t="shared" ref="AA45:AB45" si="50">INT(AA44/2)</f>
+        <f t="shared" ref="AA45:AB45" si="53">INT(AA44/2)</f>
         <v>2</v>
       </c>
       <c r="AB45" s="16">
-        <f t="shared" si="50"/>
+        <f t="shared" si="53"/>
         <v>4679</v>
       </c>
       <c r="AC45" s="16">

</xml_diff>